<commit_message>
Added grades for assesment
</commit_message>
<xml_diff>
--- a/docs/assessment/handin/papierwerk.xlsx
+++ b/docs/assessment/handin/papierwerk.xlsx
@@ -8,13 +8,13 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="Opdracht" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Userstories" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Planning" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Toetsmatrijs" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Beoordeling P1" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Beoordeling P2" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Versiebeheer" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Opdracht" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Userstories" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Planning" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Toetsmatrijs" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="Beoordeling P1" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="Beoordeling P2" sheetId="6" state="visible" r:id="rId8"/>
+    <sheet name="Versiebeheer" sheetId="7" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -959,11 +959,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
   </numFmts>
   <fonts count="19">
     <font>
@@ -1317,392 +1316,396 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="17" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="17" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="15" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="15" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="16" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="18" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="18" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="17" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="17" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="14" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="14" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1778,8 +1781,114 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1789,114 +1898,114 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="113.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="113.85"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="3"/>
+      <c r="C8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="335.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="7" t="s">
+    <row r="13" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="7"/>
-      <c r="C14" s="8" t="s">
+      <c r="B14" s="8"/>
+      <c r="C14" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="7"/>
-      <c r="C15" s="8" t="s">
+      <c r="B15" s="8"/>
+      <c r="C15" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="7"/>
-      <c r="C16" s="8" t="s">
+      <c r="B16" s="8"/>
+      <c r="C16" s="9" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="9"/>
-      <c r="C18" s="10" t="s">
+      <c r="B18" s="10"/>
+      <c r="C18" s="11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="6"/>
-      <c r="C19" s="6" t="s">
+      <c r="B19" s="7"/>
+      <c r="C19" s="7" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1915,7 +2024,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1925,681 +2034,681 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="136.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="1.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="136.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="4"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="12"/>
+      <c r="C3" s="13"/>
     </row>
     <row r="4" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="66" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="13"/>
+      <c r="C10" s="14"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="13"/>
+      <c r="C15" s="14"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="13"/>
+      <c r="C20" s="14"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="13"/>
+      <c r="C25" s="14"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="13"/>
+      <c r="C30" s="14"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="C33" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C35" s="13"/>
+      <c r="C35" s="14"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="C36" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="C37" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C38" s="0" t="s">
+      <c r="C38" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="13" t="s">
+      <c r="B40" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C40" s="13"/>
+      <c r="C40" s="14"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="0" t="s">
+      <c r="B41" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C41" s="0" t="s">
+      <c r="C41" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="0" t="s">
+      <c r="B42" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C42" s="0" t="s">
+      <c r="C42" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="0" t="s">
+      <c r="B43" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="C43" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="13" t="s">
+      <c r="B45" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C45" s="13"/>
+      <c r="C45" s="14"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="0" t="s">
+      <c r="B46" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="C46" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0" t="s">
+      <c r="B47" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C47" s="0" t="s">
+      <c r="C47" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="0" t="s">
+      <c r="B48" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C48" s="0" t="s">
+      <c r="C48" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="13" t="s">
+      <c r="B50" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C50" s="13"/>
+      <c r="C50" s="14"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="0" t="s">
+      <c r="B51" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C51" s="0" t="s">
+      <c r="C51" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="0" t="s">
+      <c r="B52" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C52" s="0" t="s">
+      <c r="C52" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="0" t="s">
+      <c r="B53" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C53" s="0" t="s">
+      <c r="C53" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="13" t="s">
+      <c r="B55" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C55" s="13"/>
+      <c r="C55" s="14"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="0" t="s">
+      <c r="B56" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C56" s="0" t="s">
+      <c r="C56" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="0" t="s">
+      <c r="B57" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C57" s="0" t="s">
+      <c r="C57" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="0" t="s">
+      <c r="B58" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C58" s="0" t="s">
+      <c r="C58" s="1" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="13" t="s">
+      <c r="B60" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="C60" s="13"/>
+      <c r="C60" s="14"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="0" t="s">
+      <c r="B61" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C61" s="0" t="s">
+      <c r="C61" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="0" t="s">
+      <c r="B62" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C62" s="0" t="s">
+      <c r="C62" s="1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="0" t="s">
+      <c r="B63" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C63" s="0" t="s">
+      <c r="C63" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="13" t="s">
+      <c r="B65" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="C65" s="13"/>
+      <c r="C65" s="14"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="0" t="s">
+      <c r="B66" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C66" s="0" t="s">
+      <c r="C66" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="0" t="s">
+      <c r="B67" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C67" s="0" t="s">
+      <c r="C67" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="0" t="s">
+      <c r="B68" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C68" s="0" t="s">
+      <c r="C68" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="13" t="s">
+      <c r="B70" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C70" s="13"/>
+      <c r="C70" s="14"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="0" t="s">
+      <c r="B71" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C71" s="0" t="s">
+      <c r="C71" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="0" t="s">
+      <c r="B72" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C72" s="0" t="s">
+      <c r="C72" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="0" t="s">
+      <c r="B73" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C73" s="0" t="s">
+      <c r="C73" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="13" t="s">
+      <c r="B75" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="C75" s="13"/>
+      <c r="C75" s="14"/>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="0" t="s">
+      <c r="B76" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C76" s="0" t="s">
+      <c r="C76" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="0" t="s">
+      <c r="B77" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C77" s="0" t="s">
+      <c r="C77" s="1" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="0" t="s">
+      <c r="B78" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C78" s="0" t="s">
+      <c r="C78" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="14" t="s">
+      <c r="A80" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="B80" s="14"/>
-      <c r="C80" s="14"/>
-      <c r="D80" s="14"/>
+      <c r="B80" s="15"/>
+      <c r="C80" s="15"/>
+      <c r="D80" s="15"/>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D81" s="15" t="s">
+      <c r="D81" s="16" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="13" t="s">
+      <c r="B82" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C82" s="16"/>
-      <c r="D82" s="17" t="n">
+      <c r="C82" s="17"/>
+      <c r="D82" s="18" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="0" t="s">
+      <c r="B83" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C83" s="0" t="s">
+      <c r="C83" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="0" t="s">
+      <c r="B84" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C84" s="0" t="s">
+      <c r="C84" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B85" s="0" t="s">
+      <c r="B85" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C85" s="0" t="s">
+      <c r="C85" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B87" s="13" t="s">
+      <c r="B87" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="C87" s="16"/>
-      <c r="D87" s="17" t="n">
+      <c r="C87" s="17"/>
+      <c r="D87" s="18" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B88" s="0" t="s">
+      <c r="B88" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C88" s="0" t="s">
+      <c r="C88" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B89" s="0" t="s">
+      <c r="B89" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C89" s="0" t="s">
+      <c r="C89" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B90" s="0" t="s">
+      <c r="B90" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C90" s="0" t="s">
+      <c r="C90" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B92" s="13" t="s">
+      <c r="B92" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="C92" s="16"/>
-      <c r="D92" s="17" t="n">
+      <c r="C92" s="17"/>
+      <c r="D92" s="18" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B93" s="0" t="s">
+      <c r="B93" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C93" s="0" t="s">
+      <c r="C93" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B94" s="0" t="s">
+      <c r="B94" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C94" s="0" t="s">
+      <c r="C94" s="1" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B95" s="0" t="s">
+      <c r="B95" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C95" s="0" t="s">
+      <c r="C95" s="1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B97" s="13" t="s">
+      <c r="B97" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="C97" s="16"/>
-      <c r="D97" s="17" t="n">
+      <c r="C97" s="17"/>
+      <c r="D97" s="18" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B98" s="0" t="s">
+      <c r="B98" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C98" s="0" t="s">
+      <c r="C98" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B99" s="0" t="s">
+      <c r="B99" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C99" s="0" t="s">
+      <c r="C99" s="1" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B100" s="0" t="s">
+      <c r="B100" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C100" s="0" t="s">
+      <c r="C100" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B102" s="13" t="s">
+      <c r="B102" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="C102" s="16"/>
-      <c r="D102" s="17" t="n">
+      <c r="C102" s="17"/>
+      <c r="D102" s="18" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B103" s="0" t="s">
+      <c r="B103" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C103" s="0" t="s">
+      <c r="C103" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B104" s="0" t="s">
+      <c r="B104" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C104" s="0" t="s">
+      <c r="C104" s="1" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B105" s="0" t="s">
+      <c r="B105" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C105" s="0" t="s">
+      <c r="C105" s="1" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B107" s="13" t="s">
+      <c r="B107" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="C107" s="16"/>
-      <c r="D107" s="17" t="n">
+      <c r="C107" s="17"/>
+      <c r="D107" s="18" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B108" s="0" t="s">
+      <c r="B108" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C108" s="0" t="s">
+      <c r="C108" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B109" s="0" t="s">
+      <c r="B109" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C109" s="0" t="s">
+      <c r="C109" s="1" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B110" s="0" t="s">
+      <c r="B110" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C110" s="0" t="s">
+      <c r="C110" s="1" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2623,7 +2732,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2633,787 +2742,787 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="1.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="74.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="1.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="1.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="6.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="5.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="6.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="25.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="74.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="77"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="4.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
     </row>
     <row r="4" customFormat="false" ht="3.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="I5" s="20" t="s">
+      <c r="I5" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="J5" s="20" t="s">
+      <c r="J5" s="21" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="21" t="n">
+      <c r="B6" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="G6" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="H6" s="21" t="s">
+      <c r="H6" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="I6" s="21" t="s">
+      <c r="I6" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="J6" s="23" t="s">
+      <c r="J6" s="24" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="F7" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="G7" s="21" t="n">
+      <c r="G7" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="I7" s="21" t="s">
+      <c r="I7" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="J7" s="23" t="s">
+      <c r="J7" s="24" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="24" t="n">
+      <c r="B8" s="25" t="n">
         <v>2</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="G8" s="24" t="n">
+      <c r="G8" s="25" t="n">
         <v>3</v>
       </c>
-      <c r="H8" s="24" t="s">
+      <c r="H8" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="I8" s="24" t="s">
+      <c r="I8" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="J8" s="26" t="s">
+      <c r="J8" s="27" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="21" t="n">
+      <c r="B9" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="G9" s="21" t="n">
+      <c r="G9" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="H9" s="21" t="s">
+      <c r="H9" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="I9" s="21" t="s">
+      <c r="I9" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="J9" s="23" t="s">
+      <c r="J9" s="24" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="28" t="n">
+      <c r="B10" s="29" t="n">
         <v>4</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="F10" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="G10" s="24" t="n">
+      <c r="G10" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="H10" s="24" t="s">
+      <c r="H10" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="I10" s="24" t="s">
+      <c r="I10" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="J10" s="26" t="s">
+      <c r="J10" s="27" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="21" t="n">
+      <c r="B11" s="22" t="n">
         <v>5</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="G11" s="21" t="n">
+      <c r="G11" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="H11" s="21" t="s">
+      <c r="H11" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="I11" s="21" t="s">
+      <c r="I11" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="J11" s="23" t="s">
+      <c r="J11" s="24" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="24" t="n">
+      <c r="B12" s="25" t="n">
         <v>6</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="F12" s="24" t="s">
+      <c r="F12" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="G12" s="24" t="n">
+      <c r="G12" s="25" t="n">
         <v>3</v>
       </c>
-      <c r="H12" s="24" t="s">
+      <c r="H12" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="I12" s="24" t="s">
+      <c r="I12" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="J12" s="26" t="s">
+      <c r="J12" s="27" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="21" t="n">
+      <c r="B13" s="22" t="n">
         <v>7</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="F13" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="G13" s="22" t="s">
+      <c r="G13" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="H13" s="21" t="s">
+      <c r="H13" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="I13" s="21" t="s">
+      <c r="I13" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="J13" s="23" t="s">
+      <c r="J13" s="24" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D14" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="F14" s="29" t="s">
+      <c r="F14" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="G14" s="30" t="s">
+      <c r="G14" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="H14" s="21" t="s">
+      <c r="H14" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="I14" s="21" t="s">
+      <c r="I14" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="J14" s="23" t="s">
+      <c r="J14" s="24" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="24" t="n">
+      <c r="B15" s="25" t="n">
         <v>8</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="E15" s="25"/>
-      <c r="F15" s="24" t="s">
+      <c r="E15" s="26"/>
+      <c r="F15" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="24" t="s">
+      <c r="G15" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="H15" s="24" t="s">
+      <c r="H15" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="I15" s="24" t="s">
+      <c r="I15" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="J15" s="26" t="s">
+      <c r="J15" s="27" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="21" t="n">
+      <c r="B16" s="22" t="n">
         <v>9</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="D16" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="E16" s="21"/>
-      <c r="F16" s="27" t="s">
+      <c r="E16" s="22"/>
+      <c r="F16" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="G16" s="27" t="s">
+      <c r="G16" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="H16" s="21" t="s">
+      <c r="H16" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="I16" s="21" t="s">
+      <c r="I16" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="J16" s="23" t="s">
+      <c r="J16" s="24" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="28" t="n">
+      <c r="B17" s="29" t="n">
         <v>10</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="D17" s="24" t="s">
+      <c r="D17" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="E17" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="F17" s="31" t="s">
+      <c r="F17" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="G17" s="24" t="n">
+      <c r="G17" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="H17" s="24" t="s">
+      <c r="H17" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="I17" s="24" t="s">
+      <c r="I17" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="J17" s="26" t="s">
+      <c r="J17" s="27" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="D18" s="32"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="24" t="s">
+      <c r="D18" s="33"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="G18" s="24" t="s">
+      <c r="G18" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="H18" s="24" t="s">
+      <c r="H18" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="I18" s="24" t="s">
+      <c r="I18" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="J18" s="26" t="s">
+      <c r="J18" s="27" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="33" t="n">
+      <c r="B19" s="34" t="n">
         <v>11</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="D19" s="33" t="s">
+      <c r="D19" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="E19" s="33" t="s">
+      <c r="E19" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="F19" s="33" t="n">
+      <c r="F19" s="34" t="n">
         <v>3</v>
       </c>
-      <c r="G19" s="33" t="n">
+      <c r="G19" s="34" t="n">
         <v>4</v>
       </c>
-      <c r="H19" s="33" t="s">
+      <c r="H19" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="I19" s="33" t="s">
+      <c r="I19" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="J19" s="34" t="s">
+      <c r="J19" s="35" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33" t="s">
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34" t="s">
         <v>154</v>
       </c>
-      <c r="E20" s="33" t="s">
+      <c r="E20" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="F20" s="33" t="s">
+      <c r="F20" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="G20" s="33" t="n">
+      <c r="G20" s="34" t="n">
         <v>1</v>
       </c>
-      <c r="H20" s="33" t="s">
+      <c r="H20" s="34" t="s">
         <v>156</v>
       </c>
-      <c r="I20" s="33" t="s">
+      <c r="I20" s="34" t="s">
         <v>157</v>
       </c>
-      <c r="J20" s="34" t="s">
+      <c r="J20" s="35" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="35" t="n">
+      <c r="B21" s="36" t="n">
         <v>12</v>
       </c>
-      <c r="C21" s="35" t="s">
+      <c r="C21" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="D21" s="35" t="s">
+      <c r="D21" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="E21" s="36" t="s">
+      <c r="E21" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="F21" s="35" t="n">
+      <c r="F21" s="36" t="n">
         <v>3</v>
       </c>
-      <c r="G21" s="35" t="n">
+      <c r="G21" s="36" t="n">
         <v>4</v>
       </c>
-      <c r="H21" s="35" t="s">
+      <c r="H21" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="I21" s="35" t="s">
+      <c r="I21" s="36" t="s">
         <v>160</v>
       </c>
-      <c r="J21" s="37" t="s">
+      <c r="J21" s="38" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="33" t="n">
+      <c r="B22" s="34" t="n">
         <v>13</v>
       </c>
-      <c r="C22" s="38" t="s">
+      <c r="C22" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="D22" s="33" t="s">
+      <c r="D22" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="E22" s="33" t="s">
+      <c r="E22" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="F22" s="33" t="n">
+      <c r="F22" s="34" t="n">
         <v>3</v>
       </c>
-      <c r="G22" s="33" t="n">
+      <c r="G22" s="34" t="n">
         <v>4</v>
       </c>
-      <c r="H22" s="33" t="s">
+      <c r="H22" s="34" t="s">
         <v>162</v>
       </c>
-      <c r="I22" s="33" t="s">
+      <c r="I22" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="J22" s="34" t="s">
+      <c r="J22" s="35" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="35" t="n">
+      <c r="B23" s="36" t="n">
         <v>14</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="D23" s="35" t="s">
+      <c r="D23" s="36" t="s">
         <v>165</v>
       </c>
-      <c r="E23" s="36" t="s">
+      <c r="E23" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="F23" s="39" t="s">
+      <c r="F23" s="40" t="s">
         <v>137</v>
       </c>
-      <c r="G23" s="39" t="s">
+      <c r="G23" s="40" t="s">
         <v>137</v>
       </c>
-      <c r="H23" s="35" t="s">
+      <c r="H23" s="36" t="s">
         <v>166</v>
       </c>
-      <c r="I23" s="35" t="s">
+      <c r="I23" s="36" t="s">
         <v>167</v>
       </c>
-      <c r="J23" s="37" t="s">
+      <c r="J23" s="38" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="33" t="n">
+      <c r="B24" s="34" t="n">
         <v>15</v>
       </c>
-      <c r="C24" s="33" t="s">
+      <c r="C24" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="D24" s="33" t="s">
+      <c r="D24" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="E24" s="33" t="s">
+      <c r="E24" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="F24" s="33" t="n">
+      <c r="F24" s="34" t="n">
         <v>3</v>
       </c>
-      <c r="G24" s="33" t="n">
+      <c r="G24" s="34" t="n">
         <v>4</v>
       </c>
-      <c r="H24" s="33" t="s">
+      <c r="H24" s="34" t="s">
         <v>169</v>
       </c>
-      <c r="I24" s="33" t="s">
+      <c r="I24" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="J24" s="34" t="s">
+      <c r="J24" s="35" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="35" t="n">
+      <c r="B25" s="36" t="n">
         <v>16</v>
       </c>
-      <c r="C25" s="35" t="s">
+      <c r="C25" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="D25" s="35" t="s">
+      <c r="D25" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="E25" s="36" t="s">
+      <c r="E25" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="F25" s="35" t="n">
+      <c r="F25" s="36" t="n">
         <v>1</v>
       </c>
-      <c r="G25" s="35" t="n">
+      <c r="G25" s="36" t="n">
         <v>1</v>
       </c>
-      <c r="H25" s="35" t="s">
+      <c r="H25" s="36" t="s">
         <v>172</v>
       </c>
-      <c r="I25" s="35" t="s">
+      <c r="I25" s="36" t="s">
         <v>173</v>
       </c>
-      <c r="J25" s="37" t="s">
+      <c r="J25" s="38" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="38" t="n">
+      <c r="B26" s="39" t="n">
         <v>17</v>
       </c>
-      <c r="C26" s="38" t="s">
+      <c r="C26" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="D26" s="33" t="s">
+      <c r="D26" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="E26" s="33" t="s">
+      <c r="E26" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="F26" s="33" t="n">
+      <c r="F26" s="34" t="n">
         <v>3</v>
       </c>
-      <c r="G26" s="40" t="s">
+      <c r="G26" s="41" t="s">
         <v>176</v>
       </c>
-      <c r="H26" s="33" t="s">
+      <c r="H26" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="I26" s="33" t="s">
+      <c r="I26" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="J26" s="34" t="s">
+      <c r="J26" s="35" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="33" t="s">
+      <c r="B27" s="39"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33" t="s">
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34" t="s">
         <v>180</v>
       </c>
-      <c r="I27" s="33"/>
-      <c r="J27" s="34" t="s">
+      <c r="I27" s="34"/>
+      <c r="J27" s="35" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="41" t="s">
+      <c r="B28" s="42" t="s">
         <v>182</v>
       </c>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="41"/>
-      <c r="I28" s="41"/>
-      <c r="J28" s="41"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="42"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="36" t="n">
+      <c r="B29" s="37" t="n">
         <v>18</v>
       </c>
-      <c r="C29" s="36" t="s">
+      <c r="C29" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="D29" s="36" t="s">
+      <c r="D29" s="37" t="s">
         <v>154</v>
       </c>
-      <c r="E29" s="36" t="s">
+      <c r="E29" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="F29" s="36" t="n">
+      <c r="F29" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="G29" s="36" t="n">
+      <c r="G29" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="H29" s="36" t="s">
+      <c r="H29" s="37" t="s">
         <v>180</v>
       </c>
-      <c r="I29" s="36"/>
-      <c r="J29" s="42" t="s">
+      <c r="I29" s="37"/>
+      <c r="J29" s="43" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="21" t="n">
+      <c r="B30" s="22" t="n">
         <v>19</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C30" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="D30" s="43" t="s">
+      <c r="D30" s="44" t="s">
         <v>184</v>
       </c>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="43"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="23"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="24"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="25" t="n">
+      <c r="B31" s="26" t="n">
         <v>20</v>
       </c>
-      <c r="C31" s="44" t="s">
+      <c r="C31" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="D31" s="45" t="s">
+      <c r="D31" s="46" t="s">
         <v>185</v>
       </c>
-      <c r="E31" s="45" t="s">
+      <c r="E31" s="46" t="s">
         <v>103</v>
       </c>
-      <c r="F31" s="45" t="n">
+      <c r="F31" s="46" t="n">
         <v>1</v>
       </c>
-      <c r="G31" s="46" t="s">
+      <c r="G31" s="47" t="s">
         <v>186</v>
       </c>
-      <c r="H31" s="45" t="s">
+      <c r="H31" s="46" t="s">
         <v>187</v>
       </c>
-      <c r="I31" s="25"/>
-      <c r="J31" s="19"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="20"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I32" s="0" t="s">
+      <c r="I32" s="1" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I33" s="0" t="s">
+      <c r="I33" s="1" t="s">
         <v>189</v>
       </c>
     </row>
@@ -3434,7 +3543,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3444,270 +3553,270 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="47" width="40.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="48" width="33.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="47" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="48" width="100.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="48" width="40.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="49" width="33.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="48" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="49" width="100.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="50" t="s">
         <v>190</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="52"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="53" t="s">
         <v>193</v>
       </c>
-      <c r="C8" s="53" t="s">
+      <c r="C8" s="54" t="s">
         <v>194</v>
       </c>
-      <c r="D8" s="52" t="s">
+      <c r="D8" s="53" t="s">
         <v>195</v>
       </c>
-      <c r="E8" s="53" t="s">
+      <c r="E8" s="54" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="54" t="s">
+      <c r="B9" s="55" t="s">
         <v>197</v>
       </c>
-      <c r="C9" s="55" t="s">
+      <c r="C9" s="56" t="s">
         <v>198</v>
       </c>
-      <c r="D9" s="56" t="n">
+      <c r="D9" s="57" t="n">
         <v>20</v>
       </c>
-      <c r="E9" s="57" t="s">
+      <c r="E9" s="58" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="54"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="55" t="s">
+      <c r="B10" s="55"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="56" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="54"/>
-      <c r="C11" s="55"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="55" t="s">
+      <c r="B11" s="55"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="56" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="54"/>
-      <c r="C12" s="58" t="s">
+      <c r="B12" s="55"/>
+      <c r="C12" s="59" t="s">
         <v>202</v>
       </c>
-      <c r="D12" s="59" t="n">
+      <c r="D12" s="60" t="n">
         <v>20</v>
       </c>
-      <c r="E12" s="60" t="s">
+      <c r="E12" s="61" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="54"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="60" t="s">
+      <c r="B13" s="55"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="61" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="54"/>
-      <c r="C14" s="58"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="58" t="s">
+      <c r="B14" s="55"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="59" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="54"/>
-      <c r="C15" s="61" t="s">
+      <c r="B15" s="55"/>
+      <c r="C15" s="62" t="s">
         <v>206</v>
       </c>
-      <c r="D15" s="56" t="n">
+      <c r="D15" s="57" t="n">
         <v>20</v>
       </c>
-      <c r="E15" s="57" t="s">
+      <c r="E15" s="58" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="54"/>
-      <c r="C16" s="61"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="62" t="s">
+      <c r="B16" s="55"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="63" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="54"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="62" t="s">
+      <c r="B17" s="55"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="63" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="54"/>
-      <c r="C18" s="61"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="62" t="s">
+      <c r="B18" s="55"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="63" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="54"/>
-      <c r="C19" s="63" t="s">
+      <c r="B19" s="55"/>
+      <c r="C19" s="64" t="s">
         <v>211</v>
       </c>
-      <c r="D19" s="59" t="n">
+      <c r="D19" s="60" t="n">
         <v>20</v>
       </c>
-      <c r="E19" s="60" t="s">
+      <c r="E19" s="61" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="54"/>
-      <c r="C20" s="63"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="60" t="s">
+      <c r="B20" s="55"/>
+      <c r="C20" s="64"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="61" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="54"/>
-      <c r="C21" s="63"/>
-      <c r="D21" s="59"/>
-      <c r="E21" s="60"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="60"/>
+      <c r="E21" s="61"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="54"/>
-      <c r="C22" s="64" t="s">
+      <c r="B22" s="55"/>
+      <c r="C22" s="65" t="s">
         <v>214</v>
       </c>
-      <c r="D22" s="56" t="n">
+      <c r="D22" s="57" t="n">
         <v>20</v>
       </c>
-      <c r="E22" s="57" t="s">
+      <c r="E22" s="58" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="54"/>
-      <c r="C23" s="64"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="57" t="s">
+      <c r="B23" s="55"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="58" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="65" t="s">
+      <c r="B25" s="66" t="s">
         <v>217</v>
       </c>
-      <c r="C25" s="66"/>
-      <c r="D25" s="67" t="n">
+      <c r="C25" s="67"/>
+      <c r="D25" s="68" t="n">
         <f aca="false">SUM(D9:D24)</f>
         <v>100</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="53" t="s">
+      <c r="C27" s="54" t="s">
         <v>218</v>
       </c>
-      <c r="D27" s="52" t="s">
+      <c r="D27" s="53" t="s">
         <v>195</v>
       </c>
-      <c r="E27" s="53" t="s">
+      <c r="E27" s="54" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C28" s="64" t="s">
+      <c r="C28" s="65" t="s">
         <v>219</v>
       </c>
-      <c r="D28" s="56" t="n">
+      <c r="D28" s="57" t="n">
         <v>100</v>
       </c>
-      <c r="E28" s="57" t="s">
+      <c r="E28" s="58" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="64"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="62" t="s">
+      <c r="C29" s="65"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="63" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="64"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="62" t="s">
+      <c r="C30" s="65"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="63" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="64"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="62" t="s">
+      <c r="C31" s="65"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="63" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="64"/>
-      <c r="D32" s="56"/>
-      <c r="E32" s="62" t="s">
+      <c r="C32" s="65"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="63" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D33" s="68"/>
+      <c r="D33" s="69"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D34" s="68"/>
+      <c r="D34" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3733,7 +3842,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3743,393 +3852,393 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="70.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="101.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="1.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="70.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="101.85"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="70" t="s">
         <v>225</v>
       </c>
-      <c r="F2" s="70" t="s">
+      <c r="F2" s="71" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F3" s="70" t="s">
+      <c r="F3" s="71" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="53" t="s">
+    <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="54" t="s">
         <v>194</v>
       </c>
-      <c r="C4" s="52" t="s">
+      <c r="C4" s="53" t="s">
         <v>195</v>
       </c>
-      <c r="D4" s="71" t="s">
+      <c r="D4" s="72" t="s">
         <v>228</v>
       </c>
-      <c r="E4" s="53" t="s">
+      <c r="E4" s="54" t="s">
         <v>229</v>
       </c>
-      <c r="F4" s="53" t="s">
+      <c r="F4" s="54" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="73" t="s">
         <v>198</v>
       </c>
-      <c r="C5" s="56" t="n">
+      <c r="C5" s="57" t="n">
         <v>20</v>
       </c>
-      <c r="D5" s="56" t="n">
+      <c r="D5" s="57" t="n">
         <v>7</v>
       </c>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="58" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="72"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="55" t="s">
+      <c r="B6" s="73"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="56" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="72"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="55" t="s">
+      <c r="B7" s="73"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="56" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="73" t="s">
+      <c r="B8" s="74" t="s">
         <v>202</v>
       </c>
-      <c r="C8" s="59" t="n">
+      <c r="C8" s="60" t="n">
         <v>20</v>
       </c>
-      <c r="D8" s="59" t="n">
+      <c r="D8" s="60" t="n">
         <v>7</v>
       </c>
-      <c r="E8" s="60" t="s">
+      <c r="E8" s="61" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="73"/>
-      <c r="C9" s="59"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="60" t="s">
+      <c r="B9" s="74"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="61" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="73"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="58" t="s">
+      <c r="B10" s="74"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="59" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="75" t="s">
         <v>206</v>
       </c>
-      <c r="C11" s="56" t="n">
+      <c r="C11" s="57" t="n">
         <v>20</v>
       </c>
-      <c r="D11" s="75" t="n">
+      <c r="D11" s="76" t="n">
         <v>7</v>
       </c>
-      <c r="E11" s="57" t="s">
+      <c r="E11" s="58" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="74"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="75"/>
-      <c r="E12" s="62" t="s">
+      <c r="B12" s="75"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="63" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="74"/>
-      <c r="C13" s="56"/>
-      <c r="D13" s="75"/>
-      <c r="E13" s="62" t="s">
+      <c r="B13" s="75"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="76"/>
+      <c r="E13" s="63" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="74"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="75"/>
-      <c r="E14" s="62" t="s">
+      <c r="B14" s="75"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="63" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="76" t="s">
+      <c r="B15" s="77" t="s">
         <v>231</v>
       </c>
-      <c r="C15" s="59" t="n">
+      <c r="C15" s="60" t="n">
         <v>20</v>
       </c>
-      <c r="D15" s="77" t="n">
+      <c r="D15" s="78" t="n">
         <v>7</v>
       </c>
-      <c r="E15" s="60" t="s">
+      <c r="E15" s="61" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="76"/>
-      <c r="C16" s="59"/>
-      <c r="D16" s="77"/>
-      <c r="E16" s="60" t="s">
+      <c r="B16" s="77"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="61" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="78" t="s">
+      <c r="B17" s="79" t="s">
         <v>232</v>
       </c>
-      <c r="C17" s="56" t="n">
+      <c r="C17" s="57" t="n">
         <v>20</v>
       </c>
-      <c r="D17" s="79" t="n">
+      <c r="D17" s="80" t="n">
         <v>7</v>
       </c>
-      <c r="E17" s="57" t="s">
+      <c r="E17" s="58" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="78"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="79"/>
-      <c r="E18" s="57" t="s">
+      <c r="B18" s="79"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="80"/>
+      <c r="E18" s="58" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="80" t="s">
+      <c r="B19" s="81" t="s">
         <v>235</v>
       </c>
-      <c r="C19" s="80"/>
-      <c r="D19" s="80"/>
-      <c r="E19" s="80"/>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="81" t="n">
+      <c r="C19" s="81"/>
+      <c r="D19" s="81"/>
+      <c r="E19" s="81"/>
+    </row>
+    <row r="20" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="82" t="n">
         <f aca="false">SUM(C5:C18)</f>
         <v>100</v>
       </c>
-      <c r="D20" s="82" t="n">
+      <c r="D20" s="83" t="n">
         <f aca="false">(D5*C5+D8*C8+D11*C11+D15*C15+D17*C17)/C20</f>
         <v>7</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="69" t="s">
+      <c r="B22" s="70" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="53" t="s">
+      <c r="B24" s="54" t="s">
         <v>237</v>
       </c>
-      <c r="C24" s="52" t="s">
+      <c r="C24" s="53" t="s">
         <v>238</v>
       </c>
-      <c r="D24" s="83" t="s">
+      <c r="D24" s="84" t="s">
         <v>239</v>
       </c>
-      <c r="E24" s="53" t="s">
+      <c r="E24" s="54" t="s">
         <v>240</v>
       </c>
-      <c r="F24" s="53" t="s">
+      <c r="F24" s="54" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C25" s="0" t="n">
+      <c r="C25" s="1" t="n">
         <v>123456</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="D25" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="E25" s="84" t="n">
+      <c r="E25" s="85" t="n">
         <f aca="false">$D$20*D25/$D$34</f>
         <v>7</v>
       </c>
-      <c r="F25" s="0" t="s">
+      <c r="F25" s="1" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C26" s="0" t="n">
+      <c r="C26" s="1" t="n">
         <v>123456</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D26" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="E26" s="84" t="n">
+      <c r="E26" s="85" t="n">
         <f aca="false">$D$20*D26/$D$34</f>
         <v>7</v>
       </c>
-      <c r="F26" s="0" t="s">
+      <c r="F26" s="1" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C27" s="0" t="n">
+      <c r="C27" s="1" t="n">
         <v>123456</v>
       </c>
-      <c r="D27" s="0" t="n">
+      <c r="D27" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="E27" s="84" t="n">
+      <c r="E27" s="85" t="n">
         <f aca="false">$D$20*D27/$D$34</f>
         <v>7</v>
       </c>
-      <c r="F27" s="0" t="s">
+      <c r="F27" s="1" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C28" s="0" t="n">
+      <c r="C28" s="1" t="n">
         <v>123456</v>
       </c>
-      <c r="D28" s="0" t="n">
+      <c r="D28" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="E28" s="84" t="n">
+      <c r="E28" s="85" t="n">
         <f aca="false">$D$20*D28/$D$34</f>
         <v>7</v>
       </c>
-      <c r="F28" s="0" t="s">
+      <c r="F28" s="1" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C29" s="0" t="n">
+      <c r="C29" s="1" t="n">
         <v>123456</v>
       </c>
-      <c r="D29" s="0" t="n">
+      <c r="D29" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="E29" s="84" t="n">
+      <c r="E29" s="85" t="n">
         <f aca="false">$D$20*D29/$D$34</f>
         <v>7</v>
       </c>
-      <c r="F29" s="0" t="s">
+      <c r="F29" s="1" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C30" s="0" t="n">
+      <c r="C30" s="1" t="n">
         <v>123456</v>
       </c>
-      <c r="D30" s="0" t="n">
+      <c r="D30" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="E30" s="84" t="n">
+      <c r="E30" s="85" t="n">
         <f aca="false">$D$20*D30/$D$34</f>
         <v>7</v>
       </c>
-      <c r="F30" s="0" t="s">
+      <c r="F30" s="1" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C31" s="0" t="n">
+      <c r="C31" s="1" t="n">
         <v>123456</v>
       </c>
-      <c r="D31" s="0" t="n">
+      <c r="D31" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="E31" s="84" t="n">
+      <c r="E31" s="85" t="n">
         <f aca="false">$D$20*D31/$D$34</f>
         <v>7</v>
       </c>
-      <c r="F31" s="0" t="s">
+      <c r="F31" s="1" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C32" s="0" t="n">
+      <c r="C32" s="1" t="n">
         <v>123456</v>
       </c>
-      <c r="D32" s="0" t="n">
+      <c r="D32" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="E32" s="84" t="n">
+      <c r="E32" s="85" t="n">
         <f aca="false">$D$20*D32/$D$34</f>
         <v>7</v>
       </c>
-      <c r="F32" s="0" t="s">
+      <c r="F32" s="1" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="85" t="s">
+      <c r="C34" s="86" t="s">
         <v>244</v>
       </c>
-      <c r="D34" s="0" t="n">
+      <c r="D34" s="1" t="n">
         <f aca="false">AVERAGE(D25:D32)</f>
         <v>7</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="1" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="1" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="1" t="s">
         <v>247</v>
       </c>
     </row>
@@ -4163,620 +4272,620 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="B2:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E42" activeCellId="0" sqref="E42"/>
+      <selection pane="topLeft" activeCell="E53" activeCellId="0" sqref="E53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="70.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="101.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="1.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="70.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="101.85"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="70" t="s">
         <v>248</v>
       </c>
-      <c r="F2" s="70" t="s">
+      <c r="F2" s="71" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F3" s="70" t="s">
+      <c r="F3" s="71" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="53" t="s">
+    <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="54" t="s">
         <v>194</v>
       </c>
-      <c r="C4" s="52" t="s">
+      <c r="C4" s="53" t="s">
         <v>195</v>
       </c>
-      <c r="D4" s="71" t="s">
+      <c r="D4" s="72" t="s">
         <v>249</v>
       </c>
-      <c r="E4" s="53" t="s">
+      <c r="E4" s="54" t="s">
         <v>229</v>
       </c>
-      <c r="F4" s="53" t="s">
+      <c r="F4" s="54" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="73" t="s">
         <v>198</v>
       </c>
-      <c r="C5" s="56" t="n">
+      <c r="C5" s="57" t="n">
         <v>20</v>
       </c>
-      <c r="D5" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="57" t="s">
+      <c r="D5" s="80" t="n">
+        <v>9</v>
+      </c>
+      <c r="E5" s="58" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="72"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="55" t="s">
+      <c r="B6" s="73"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="56" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="72"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="55" t="s">
+      <c r="B7" s="73"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="80"/>
+      <c r="E7" s="56" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="73" t="s">
+      <c r="B8" s="74" t="s">
         <v>202</v>
       </c>
-      <c r="C8" s="59" t="n">
+      <c r="C8" s="60" t="n">
         <v>20</v>
       </c>
-      <c r="D8" s="77" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="60" t="s">
+      <c r="D8" s="78" t="n">
+        <v>9</v>
+      </c>
+      <c r="E8" s="61" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="73"/>
-      <c r="C9" s="59"/>
-      <c r="D9" s="77"/>
-      <c r="E9" s="60" t="s">
+      <c r="B9" s="74"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="61" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="73"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="77"/>
-      <c r="E10" s="58" t="s">
+      <c r="B10" s="74"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="59" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="75" t="s">
         <v>206</v>
       </c>
-      <c r="C11" s="56" t="n">
+      <c r="C11" s="57" t="n">
         <v>20</v>
       </c>
-      <c r="D11" s="86" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" s="57" t="s">
+      <c r="D11" s="87" t="n">
+        <v>9</v>
+      </c>
+      <c r="E11" s="58" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="74"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="62" t="s">
+      <c r="B12" s="75"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="87"/>
+      <c r="E12" s="63" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="74"/>
-      <c r="C13" s="56"/>
-      <c r="D13" s="86"/>
-      <c r="E13" s="62" t="s">
+      <c r="B13" s="75"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="87"/>
+      <c r="E13" s="63" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="74"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="86"/>
-      <c r="E14" s="62" t="s">
+      <c r="B14" s="75"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="87"/>
+      <c r="E14" s="63" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="76" t="s">
+      <c r="B15" s="77" t="s">
         <v>231</v>
       </c>
-      <c r="C15" s="59" t="n">
+      <c r="C15" s="60" t="n">
         <v>20</v>
       </c>
-      <c r="D15" s="77" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" s="60" t="s">
+      <c r="D15" s="78" t="n">
+        <v>10</v>
+      </c>
+      <c r="E15" s="61" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="76"/>
-      <c r="C16" s="59"/>
-      <c r="D16" s="77"/>
-      <c r="E16" s="60" t="s">
+      <c r="B16" s="77"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="61" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="78" t="s">
+      <c r="B17" s="79" t="s">
         <v>232</v>
       </c>
-      <c r="C17" s="56" t="n">
+      <c r="C17" s="57" t="n">
         <v>20</v>
       </c>
-      <c r="D17" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="E17" s="57" t="s">
+      <c r="D17" s="80" t="n">
+        <v>9</v>
+      </c>
+      <c r="E17" s="58" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="78"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="79"/>
-      <c r="E18" s="57" t="s">
+    <row r="18" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="79"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="80"/>
+      <c r="E18" s="58" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="80" t="s">
+      <c r="B19" s="81" t="s">
         <v>251</v>
       </c>
-      <c r="C19" s="80"/>
-      <c r="D19" s="80"/>
-      <c r="E19" s="80"/>
-    </row>
-    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="81" t="n">
+      <c r="C19" s="81"/>
+      <c r="D19" s="81"/>
+      <c r="E19" s="81"/>
+    </row>
+    <row r="20" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="82" t="n">
         <f aca="false">SUM(C5:C18)</f>
         <v>100</v>
       </c>
-      <c r="D20" s="82" t="n">
+      <c r="D20" s="83" t="n">
         <f aca="false">(D5*C5+D8*C8+D11*C11+D15*C15+D17*C17)/C20</f>
-        <v>0</v>
+        <v>9.2</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="70" t="s">
+      <c r="B22" s="71" t="s">
         <v>252</v>
       </c>
-      <c r="F22" s="87" t="s">
+      <c r="F22" s="88" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="70" t="s">
+      <c r="B23" s="71" t="s">
         <v>254</v>
       </c>
-      <c r="F23" s="88"/>
+      <c r="F23" s="89"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F24" s="88"/>
+      <c r="F24" s="89"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C25" s="89" t="s">
+      <c r="C25" s="90" t="s">
         <v>255</v>
       </c>
-      <c r="D25" s="89"/>
-      <c r="F25" s="88"/>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="90" t="s">
+      <c r="D25" s="90"/>
+      <c r="F25" s="89"/>
+    </row>
+    <row r="26" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="91" t="s">
         <v>256</v>
       </c>
-      <c r="C26" s="89" t="s">
+      <c r="C26" s="90" t="s">
         <v>257</v>
       </c>
-      <c r="D26" s="89" t="s">
+      <c r="D26" s="90" t="s">
         <v>258</v>
       </c>
-      <c r="E26" s="91" t="s">
+      <c r="E26" s="92" t="s">
         <v>259</v>
       </c>
-      <c r="F26" s="88"/>
+      <c r="F26" s="89"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0" t="n">
+      <c r="B27" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E27" s="0" t="s">
+      <c r="E27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F27" s="88"/>
+      <c r="F27" s="89"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="n">
+      <c r="B28" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E28" s="0" t="s">
+      <c r="E28" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F28" s="88"/>
+      <c r="F28" s="89"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="n">
+      <c r="B29" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E29" s="0" t="s">
+      <c r="E29" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="88"/>
+      <c r="F29" s="89"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0" t="n">
+      <c r="B30" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C30" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E30" s="0" t="s">
+      <c r="E30" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F30" s="88"/>
+      <c r="F30" s="89"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0" t="n">
+      <c r="B31" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E31" s="0" t="s">
+      <c r="E31" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F31" s="88"/>
+      <c r="F31" s="89"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="n">
+      <c r="B32" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E32" s="0" t="s">
+      <c r="E32" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F32" s="88"/>
+      <c r="F32" s="89"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0" t="n">
+      <c r="B33" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="C33" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E33" s="0" t="s">
+      <c r="E33" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="F33" s="88"/>
+      <c r="F33" s="89"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0" t="n">
+      <c r="B34" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="C34" s="0" t="s">
+      <c r="C34" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E34" s="0" t="s">
+      <c r="E34" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F34" s="88"/>
+      <c r="F34" s="89"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0" t="n">
+      <c r="B35" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="C35" s="0" t="s">
+      <c r="C35" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E35" s="0" t="s">
+      <c r="E35" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F35" s="88"/>
+      <c r="F35" s="89"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="0" t="n">
+      <c r="B36" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="C36" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E36" s="0" t="s">
+      <c r="E36" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F36" s="88"/>
+      <c r="F36" s="89"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="0" t="n">
+      <c r="B37" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="C37" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E37" s="0" t="s">
+      <c r="E37" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F37" s="88"/>
+      <c r="F37" s="89"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="0" t="n">
+      <c r="B38" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="C38" s="0" t="s">
+      <c r="C38" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E38" s="0" t="s">
+      <c r="E38" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F38" s="88"/>
+      <c r="F38" s="89"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="0" t="n">
+      <c r="B39" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="C39" s="0" t="s">
+      <c r="C39" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E39" s="0" t="s">
+      <c r="E39" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F39" s="88"/>
+      <c r="F39" s="89"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="0" t="n">
+      <c r="B40" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="C40" s="0" t="s">
+      <c r="C40" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E40" s="0" t="s">
+      <c r="E40" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F40" s="88"/>
+      <c r="F40" s="89"/>
     </row>
     <row r="41" customFormat="false" ht="5.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B41" s="92"/>
-      <c r="C41" s="92"/>
-      <c r="D41" s="92"/>
-      <c r="E41" s="92"/>
-      <c r="F41" s="88"/>
+      <c r="B41" s="93"/>
+      <c r="C41" s="93"/>
+      <c r="D41" s="93"/>
+      <c r="E41" s="93"/>
+      <c r="F41" s="89"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="0" t="n">
+      <c r="B42" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="C42" s="0" t="s">
+      <c r="C42" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E42" s="0" t="s">
+      <c r="E42" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="F42" s="88"/>
+      <c r="F42" s="89"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="0" t="n">
+      <c r="B43" s="1" t="n">
         <v>102</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="C43" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="E43" s="0" t="s">
+      <c r="E43" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="F43" s="88"/>
+      <c r="F43" s="89"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="0" t="n">
+      <c r="B44" s="1" t="n">
         <v>103</v>
       </c>
-      <c r="C44" s="0" t="s">
+      <c r="C44" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="E44" s="0" t="s">
+      <c r="E44" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="F44" s="88"/>
+      <c r="F44" s="89"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="0" t="n">
+      <c r="B45" s="1" t="n">
         <v>104</v>
       </c>
-      <c r="C45" s="0" t="s">
+      <c r="C45" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="E45" s="0" t="s">
+      <c r="E45" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="F45" s="88"/>
+      <c r="F45" s="89"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="0" t="n">
+      <c r="B46" s="1" t="n">
         <v>105</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="C46" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="E46" s="0" t="s">
+      <c r="E46" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="F46" s="88"/>
+      <c r="F46" s="89"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0" t="n">
+      <c r="B47" s="1" t="n">
         <v>106</v>
       </c>
-      <c r="C47" s="0" t="s">
+      <c r="C47" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E47" s="0" t="s">
+      <c r="E47" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="F47" s="88"/>
+      <c r="F47" s="89"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="69" t="s">
+      <c r="B49" s="70" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="53" t="s">
+      <c r="B51" s="54" t="s">
         <v>237</v>
       </c>
-      <c r="C51" s="52" t="s">
+      <c r="C51" s="53" t="s">
         <v>238</v>
       </c>
-      <c r="D51" s="83" t="s">
+      <c r="D51" s="84" t="s">
         <v>239</v>
       </c>
-      <c r="E51" s="53" t="s">
+      <c r="E51" s="54" t="s">
         <v>270</v>
       </c>
-      <c r="F51" s="53" t="s">
+      <c r="F51" s="54" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="0" t="s">
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="C52" s="0" t="n">
+      <c r="C52" s="1" t="n">
         <v>2183499</v>
       </c>
-      <c r="D52" s="0" t="n">
+      <c r="D52" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="E52" s="84" t="n">
+      <c r="E52" s="85" t="n">
         <f aca="false">$D$20*D52/$D$58</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="0" t="s">
+        <v>10.0821917808219</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="C53" s="0" t="n">
+      <c r="C53" s="1" t="n">
         <v>2184122</v>
       </c>
-      <c r="D53" s="0" t="n">
+      <c r="D53" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="E53" s="84" t="n">
+      <c r="E53" s="85" t="n">
         <f aca="false">$D$20*D53/$D$58</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="0" t="s">
+        <v>10.0821917808219</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="C54" s="0" t="n">
+      <c r="C54" s="1" t="n">
         <v>2184441</v>
       </c>
-      <c r="D54" s="0" t="n">
+      <c r="D54" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="E54" s="84" t="n">
+      <c r="E54" s="85" t="n">
         <f aca="false">$D$20*D54/$D$58</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="0" t="s">
+        <v>10.0821917808219</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="C55" s="0" t="n">
+      <c r="C55" s="1" t="n">
         <v>2177643</v>
       </c>
-      <c r="D55" s="0" t="n">
+      <c r="D55" s="1" t="n">
         <v>6.5</v>
       </c>
-      <c r="E55" s="84" t="n">
+      <c r="E55" s="85" t="n">
         <f aca="false">$D$20*D55/$D$58</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="0" t="s">
+        <v>8.19178082191781</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="C56" s="0" t="n">
+      <c r="C56" s="1" t="n">
         <v>2154689</v>
       </c>
-      <c r="D56" s="0" t="n">
+      <c r="D56" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="E56" s="84" t="n">
+      <c r="E56" s="85" t="n">
         <f aca="false">$D$20*D56/$D$58</f>
-        <v>0</v>
+        <v>7.56164383561644</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C58" s="85" t="s">
+      <c r="C58" s="86" t="s">
         <v>244</v>
       </c>
-      <c r="D58" s="0" t="n">
+      <c r="D58" s="1" t="n">
         <f aca="false">AVERAGE(D52:D56)</f>
         <v>7.3</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="0" t="s">
+      <c r="B60" s="1" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="0" t="s">
+      <c r="B61" s="1" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="0" t="s">
+      <c r="B62" s="1" t="s">
         <v>247</v>
       </c>
     </row>
@@ -4815,7 +4924,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -4825,54 +4934,54 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="122.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="122.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="93" t="s">
+      <c r="B2" s="94" t="s">
         <v>277</v>
       </c>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
     </row>
     <row r="3" customFormat="false" ht="5.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="70" t="s">
         <v>278</v>
       </c>
-      <c r="C4" s="69" t="s">
+      <c r="C4" s="70" t="s">
         <v>279</v>
       </c>
-      <c r="D4" s="69" t="s">
+      <c r="D4" s="70" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="94" t="n">
+      <c r="B5" s="95" t="n">
         <v>45527</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="95" t="s">
+      <c r="D5" s="96" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="96"/>
-      <c r="C7" s="85"/>
+      <c r="B7" s="97"/>
+      <c r="C7" s="86"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="94"/>
+      <c r="B8" s="95"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Revert "merging documents into development to remove unnecessary files"
</commit_message>
<xml_diff>
--- a/docs/assessment/handin/papierwerk.xlsx
+++ b/docs/assessment/handin/papierwerk.xlsx
@@ -8,13 +8,13 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="Opdracht" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Userstories" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="Planning" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="Toetsmatrijs" sheetId="4" state="visible" r:id="rId6"/>
-    <sheet name="Beoordeling P1" sheetId="5" state="visible" r:id="rId7"/>
-    <sheet name="Beoordeling P2" sheetId="6" state="visible" r:id="rId8"/>
-    <sheet name="Versiebeheer" sheetId="7" state="visible" r:id="rId9"/>
+    <sheet name="Opdracht" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Userstories" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Planning" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Toetsmatrijs" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Beoordeling P1" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Beoordeling P2" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Versiebeheer" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -959,10 +959,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="m/d/yyyy"/>
   </numFmts>
   <fonts count="19">
     <font>
@@ -1316,396 +1317,392 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="97">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="17" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="15" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="18" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="17" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="14" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="17" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="15" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="16" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="18" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="17" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="14" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1781,114 +1778,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
-  <a:themeElements>
-    <a:clrScheme name="LibreOffice">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="ffffff"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="18a303"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="0369a3"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a33e03"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8e03a3"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="c99c00"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="c9211e"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ee"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="551a8b"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1898,114 +1789,114 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="113.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="113.85"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="335.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="5"/>
+      <c r="C9" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="8" t="s">
+    <row r="13" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="8"/>
-      <c r="C14" s="9" t="s">
+      <c r="B14" s="7"/>
+      <c r="C14" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="8"/>
-      <c r="C15" s="9" t="s">
+      <c r="B15" s="7"/>
+      <c r="C15" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="8"/>
-      <c r="C16" s="9" t="s">
+      <c r="B16" s="7"/>
+      <c r="C16" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="10"/>
-      <c r="C18" s="11" t="s">
+      <c r="B18" s="9"/>
+      <c r="C18" s="10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="7"/>
-      <c r="C19" s="7" t="s">
+      <c r="B19" s="6"/>
+      <c r="C19" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2024,7 +1915,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2034,681 +1925,681 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="1.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="136.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="136.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="13"/>
+      <c r="C3" s="12"/>
     </row>
     <row r="4" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="66" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="14"/>
+      <c r="C10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="0" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="0" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="0" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="14"/>
+      <c r="C15" s="13"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="0" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="0" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="0" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="14"/>
+      <c r="C20" s="13"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="0" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="0" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="0" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="14"/>
+      <c r="C25" s="13"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="0" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="0" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="0" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="14"/>
+      <c r="C30" s="13"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="0" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="0" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="0" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C35" s="14"/>
+      <c r="C35" s="13"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="0" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="0" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="0" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C40" s="14"/>
+      <c r="C40" s="13"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="0" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="0" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" s="0" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="14" t="s">
+      <c r="B45" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C45" s="14"/>
+      <c r="C45" s="13"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" s="0" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" s="0" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="0" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="14" t="s">
+      <c r="B50" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C50" s="14"/>
+      <c r="C50" s="13"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" s="0" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" s="0" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="1" t="s">
+      <c r="B53" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" s="0" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="14" t="s">
+      <c r="B55" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="C55" s="14"/>
+      <c r="C55" s="13"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="1" t="s">
+      <c r="B56" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" s="0" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="1" t="s">
+      <c r="B57" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" s="0" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="0" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="14" t="s">
+      <c r="B60" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C60" s="14"/>
+      <c r="C60" s="13"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" s="0" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="1" t="s">
+      <c r="B62" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" s="0" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" s="0" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="14" t="s">
+      <c r="B65" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C65" s="14"/>
+      <c r="C65" s="13"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="1" t="s">
+      <c r="B66" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C66" s="0" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="1" t="s">
+      <c r="B67" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C67" s="0" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="1" t="s">
+      <c r="B68" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C68" s="0" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="14" t="s">
+      <c r="B70" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C70" s="14"/>
+      <c r="C70" s="13"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="1" t="s">
+      <c r="B71" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C71" s="0" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="1" t="s">
+      <c r="B72" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C72" s="0" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="1" t="s">
+      <c r="B73" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C73" s="0" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="14" t="s">
+      <c r="B75" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C75" s="14"/>
+      <c r="C75" s="13"/>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="1" t="s">
+      <c r="B76" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C76" s="0" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="1" t="s">
+      <c r="B77" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C77" s="0" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="1" t="s">
+      <c r="B78" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C78" s="0" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="15" t="s">
+      <c r="A80" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="B80" s="15"/>
-      <c r="C80" s="15"/>
-      <c r="D80" s="15"/>
+      <c r="B80" s="14"/>
+      <c r="C80" s="14"/>
+      <c r="D80" s="14"/>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D81" s="16" t="s">
+      <c r="D81" s="15" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="14" t="s">
+      <c r="B82" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="C82" s="17"/>
-      <c r="D82" s="18" t="n">
+      <c r="C82" s="16"/>
+      <c r="D82" s="17" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="1" t="s">
+      <c r="B83" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C83" s="0" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="1" t="s">
+      <c r="B84" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C84" s="0" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B85" s="1" t="s">
+      <c r="B85" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C85" s="0" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B87" s="14" t="s">
+      <c r="B87" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="C87" s="17"/>
-      <c r="D87" s="18" t="n">
+      <c r="C87" s="16"/>
+      <c r="D87" s="17" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B88" s="1" t="s">
+      <c r="B88" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C88" s="0" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B89" s="1" t="s">
+      <c r="B89" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C89" s="0" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B90" s="1" t="s">
+      <c r="B90" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C90" s="0" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B92" s="14" t="s">
+      <c r="B92" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="C92" s="17"/>
-      <c r="D92" s="18" t="n">
+      <c r="C92" s="16"/>
+      <c r="D92" s="17" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B93" s="1" t="s">
+      <c r="B93" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="C93" s="0" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B94" s="1" t="s">
+      <c r="B94" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="C94" s="0" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B95" s="1" t="s">
+      <c r="B95" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C95" s="0" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B97" s="14" t="s">
+      <c r="B97" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C97" s="17"/>
-      <c r="D97" s="18" t="n">
+      <c r="C97" s="16"/>
+      <c r="D97" s="17" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B98" s="1" t="s">
+      <c r="B98" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="C98" s="0" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B99" s="1" t="s">
+      <c r="B99" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C99" s="0" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B100" s="1" t="s">
+      <c r="B100" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="C100" s="0" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B102" s="14" t="s">
+      <c r="B102" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="C102" s="17"/>
-      <c r="D102" s="18" t="n">
+      <c r="C102" s="16"/>
+      <c r="D102" s="17" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B103" s="1" t="s">
+      <c r="B103" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="C103" s="0" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B104" s="1" t="s">
+      <c r="B104" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="C104" s="0" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B105" s="1" t="s">
+      <c r="B105" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="C105" s="0" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B107" s="14" t="s">
+      <c r="B107" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="C107" s="17"/>
-      <c r="D107" s="18" t="n">
+      <c r="C107" s="16"/>
+      <c r="D107" s="17" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B108" s="1" t="s">
+      <c r="B108" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C108" s="1" t="s">
+      <c r="C108" s="0" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B109" s="1" t="s">
+      <c r="B109" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C109" s="1" t="s">
+      <c r="C109" s="0" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B110" s="1" t="s">
+      <c r="B110" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C110" s="1" t="s">
+      <c r="C110" s="0" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2732,7 +2623,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2742,787 +2633,787 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="1.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="1.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="6.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="5.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="6.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="25.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="74.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="1.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="74.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="77"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="4.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
     </row>
     <row r="4" customFormat="false" ht="3.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="G5" s="21" t="s">
+      <c r="G5" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="H5" s="21" t="s">
+      <c r="H5" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="I5" s="21" t="s">
+      <c r="I5" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="J5" s="21" t="s">
+      <c r="J5" s="20" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="22" t="n">
+      <c r="B6" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="F6" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="H6" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="I6" s="22" t="s">
+      <c r="I6" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="J6" s="24" t="s">
+      <c r="J6" s="23" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="G7" s="22" t="n">
+      <c r="G7" s="21" t="n">
         <v>3</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="H7" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="I7" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="J7" s="24" t="s">
+      <c r="J7" s="23" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="25" t="n">
+      <c r="B8" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="F8" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="G8" s="25" t="n">
+      <c r="G8" s="24" t="n">
         <v>3</v>
       </c>
-      <c r="H8" s="25" t="s">
+      <c r="H8" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="I8" s="25" t="s">
+      <c r="I8" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="J8" s="27" t="s">
+      <c r="J8" s="26" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="22" t="n">
+      <c r="B9" s="21" t="n">
         <v>3</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="F9" s="22" t="s">
+      <c r="F9" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="G9" s="22" t="n">
+      <c r="G9" s="21" t="n">
         <v>3</v>
       </c>
-      <c r="H9" s="22" t="s">
+      <c r="H9" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="I9" s="22" t="s">
+      <c r="I9" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="J9" s="24" t="s">
+      <c r="J9" s="23" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="29" t="n">
+      <c r="B10" s="28" t="n">
         <v>4</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="E10" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="F10" s="25" t="s">
+      <c r="F10" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="G10" s="25" t="n">
+      <c r="G10" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="H10" s="25" t="s">
+      <c r="H10" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="I10" s="25" t="s">
+      <c r="I10" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="J10" s="27" t="s">
+      <c r="J10" s="26" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="22" t="n">
+      <c r="B11" s="21" t="n">
         <v>5</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="F11" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="G11" s="22" t="n">
+      <c r="G11" s="21" t="n">
         <v>3</v>
       </c>
-      <c r="H11" s="22" t="s">
+      <c r="H11" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="I11" s="22" t="s">
+      <c r="I11" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="J11" s="24" t="s">
+      <c r="J11" s="23" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="25" t="n">
+      <c r="B12" s="24" t="n">
         <v>6</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D12" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="E12" s="26" t="s">
+      <c r="E12" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="F12" s="25" t="s">
+      <c r="F12" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="G12" s="25" t="n">
+      <c r="G12" s="24" t="n">
         <v>3</v>
       </c>
-      <c r="H12" s="25" t="s">
+      <c r="H12" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="I12" s="25" t="s">
+      <c r="I12" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="J12" s="27" t="s">
+      <c r="J12" s="26" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="22" t="n">
+      <c r="B13" s="21" t="n">
         <v>7</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="F13" s="22" t="s">
+      <c r="F13" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="G13" s="23" t="s">
+      <c r="G13" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="H13" s="22" t="s">
+      <c r="H13" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="I13" s="22" t="s">
+      <c r="I13" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="J13" s="24" t="s">
+      <c r="J13" s="23" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="E14" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="F14" s="30" t="s">
+      <c r="F14" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="G14" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="H14" s="22" t="s">
+      <c r="H14" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="I14" s="22" t="s">
+      <c r="I14" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="J14" s="24" t="s">
+      <c r="J14" s="23" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="25" t="n">
+      <c r="B15" s="24" t="n">
         <v>8</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="E15" s="26"/>
-      <c r="F15" s="25" t="s">
+      <c r="E15" s="25"/>
+      <c r="F15" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="25" t="s">
+      <c r="G15" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="H15" s="25" t="s">
+      <c r="H15" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="I15" s="25" t="s">
+      <c r="I15" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="J15" s="27" t="s">
+      <c r="J15" s="26" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="22" t="n">
+      <c r="B16" s="21" t="n">
         <v>9</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="E16" s="22"/>
-      <c r="F16" s="28" t="s">
+      <c r="E16" s="21"/>
+      <c r="F16" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="G16" s="28" t="s">
+      <c r="G16" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="I16" s="22" t="s">
+      <c r="I16" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="J16" s="24" t="s">
+      <c r="J16" s="23" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="29" t="n">
+      <c r="B17" s="28" t="n">
         <v>10</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="D17" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="E17" s="26" t="s">
+      <c r="E17" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="F17" s="32" t="s">
+      <c r="F17" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="G17" s="25" t="n">
+      <c r="G17" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="H17" s="25" t="s">
+      <c r="H17" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="I17" s="25" t="s">
+      <c r="I17" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="J17" s="27" t="s">
+      <c r="J17" s="26" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="C18" s="25" t="s">
+      <c r="C18" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="D18" s="33"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="25" t="s">
+      <c r="D18" s="32"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="G18" s="25" t="s">
+      <c r="G18" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="H18" s="25" t="s">
+      <c r="H18" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="I18" s="25" t="s">
+      <c r="I18" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="J18" s="27" t="s">
+      <c r="J18" s="26" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="34" t="n">
+      <c r="B19" s="33" t="n">
         <v>11</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="D19" s="34" t="s">
+      <c r="D19" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="E19" s="34" t="s">
+      <c r="E19" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="F19" s="34" t="n">
+      <c r="F19" s="33" t="n">
         <v>3</v>
       </c>
-      <c r="G19" s="34" t="n">
+      <c r="G19" s="33" t="n">
         <v>4</v>
       </c>
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="I19" s="34" t="s">
+      <c r="I19" s="33" t="s">
         <v>152</v>
       </c>
-      <c r="J19" s="35" t="s">
+      <c r="J19" s="34" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34" t="s">
+      <c r="B20" s="33"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33" t="s">
         <v>154</v>
       </c>
-      <c r="E20" s="34" t="s">
+      <c r="E20" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="F20" s="34" t="s">
+      <c r="F20" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="G20" s="34" t="n">
+      <c r="G20" s="33" t="n">
         <v>1</v>
       </c>
-      <c r="H20" s="34" t="s">
+      <c r="H20" s="33" t="s">
         <v>156</v>
       </c>
-      <c r="I20" s="34" t="s">
+      <c r="I20" s="33" t="s">
         <v>157</v>
       </c>
-      <c r="J20" s="35" t="s">
+      <c r="J20" s="34" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="36" t="n">
+      <c r="B21" s="35" t="n">
         <v>12</v>
       </c>
-      <c r="C21" s="36" t="s">
+      <c r="C21" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="D21" s="36" t="s">
+      <c r="D21" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="E21" s="37" t="s">
+      <c r="E21" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="F21" s="36" t="n">
+      <c r="F21" s="35" t="n">
         <v>3</v>
       </c>
-      <c r="G21" s="36" t="n">
+      <c r="G21" s="35" t="n">
         <v>4</v>
       </c>
-      <c r="H21" s="36" t="s">
+      <c r="H21" s="35" t="s">
         <v>159</v>
       </c>
-      <c r="I21" s="36" t="s">
+      <c r="I21" s="35" t="s">
         <v>160</v>
       </c>
-      <c r="J21" s="38" t="s">
+      <c r="J21" s="37" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="34" t="n">
+      <c r="B22" s="33" t="n">
         <v>13</v>
       </c>
-      <c r="C22" s="39" t="s">
+      <c r="C22" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="D22" s="34" t="s">
+      <c r="D22" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="E22" s="34" t="s">
+      <c r="E22" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="F22" s="34" t="n">
+      <c r="F22" s="33" t="n">
         <v>3</v>
       </c>
-      <c r="G22" s="34" t="n">
+      <c r="G22" s="33" t="n">
         <v>4</v>
       </c>
-      <c r="H22" s="34" t="s">
+      <c r="H22" s="33" t="s">
         <v>162</v>
       </c>
-      <c r="I22" s="34" t="s">
+      <c r="I22" s="33" t="s">
         <v>163</v>
       </c>
-      <c r="J22" s="35" t="s">
+      <c r="J22" s="34" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="36" t="n">
+      <c r="B23" s="35" t="n">
         <v>14</v>
       </c>
-      <c r="C23" s="36" t="s">
+      <c r="C23" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="D23" s="36" t="s">
+      <c r="D23" s="35" t="s">
         <v>165</v>
       </c>
-      <c r="E23" s="37" t="s">
+      <c r="E23" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="F23" s="40" t="s">
+      <c r="F23" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="G23" s="40" t="s">
+      <c r="G23" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="H23" s="36" t="s">
+      <c r="H23" s="35" t="s">
         <v>166</v>
       </c>
-      <c r="I23" s="36" t="s">
+      <c r="I23" s="35" t="s">
         <v>167</v>
       </c>
-      <c r="J23" s="38" t="s">
+      <c r="J23" s="37" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="34" t="n">
+      <c r="B24" s="33" t="n">
         <v>15</v>
       </c>
-      <c r="C24" s="34" t="s">
+      <c r="C24" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="D24" s="34" t="s">
+      <c r="D24" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="E24" s="34" t="s">
+      <c r="E24" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="F24" s="34" t="n">
+      <c r="F24" s="33" t="n">
         <v>3</v>
       </c>
-      <c r="G24" s="34" t="n">
+      <c r="G24" s="33" t="n">
         <v>4</v>
       </c>
-      <c r="H24" s="34" t="s">
+      <c r="H24" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="I24" s="34" t="s">
+      <c r="I24" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="J24" s="35" t="s">
+      <c r="J24" s="34" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="36" t="n">
+      <c r="B25" s="35" t="n">
         <v>16</v>
       </c>
-      <c r="C25" s="36" t="s">
+      <c r="C25" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="D25" s="36" t="s">
+      <c r="D25" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="E25" s="37" t="s">
+      <c r="E25" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="F25" s="36" t="n">
+      <c r="F25" s="35" t="n">
         <v>1</v>
       </c>
-      <c r="G25" s="36" t="n">
+      <c r="G25" s="35" t="n">
         <v>1</v>
       </c>
-      <c r="H25" s="36" t="s">
+      <c r="H25" s="35" t="s">
         <v>172</v>
       </c>
-      <c r="I25" s="36" t="s">
+      <c r="I25" s="35" t="s">
         <v>173</v>
       </c>
-      <c r="J25" s="38" t="s">
+      <c r="J25" s="37" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="39" t="n">
+      <c r="B26" s="38" t="n">
         <v>17</v>
       </c>
-      <c r="C26" s="39" t="s">
+      <c r="C26" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="D26" s="34" t="s">
+      <c r="D26" s="33" t="s">
         <v>175</v>
       </c>
-      <c r="E26" s="34" t="s">
+      <c r="E26" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="F26" s="34" t="n">
+      <c r="F26" s="33" t="n">
         <v>3</v>
       </c>
-      <c r="G26" s="41" t="s">
+      <c r="G26" s="40" t="s">
         <v>176</v>
       </c>
-      <c r="H26" s="34" t="s">
+      <c r="H26" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="I26" s="34" t="s">
+      <c r="I26" s="33" t="s">
         <v>177</v>
       </c>
-      <c r="J26" s="35" t="s">
+      <c r="J26" s="34" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="39"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="34" t="s">
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="33" t="s">
         <v>179</v>
       </c>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34" t="s">
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="33" t="s">
         <v>180</v>
       </c>
-      <c r="I27" s="34"/>
-      <c r="J27" s="35" t="s">
+      <c r="I27" s="33"/>
+      <c r="J27" s="34" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="42" t="s">
+      <c r="B28" s="41" t="s">
         <v>182</v>
       </c>
-      <c r="C28" s="42"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="42"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="42"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
+      <c r="G28" s="41"/>
+      <c r="H28" s="41"/>
+      <c r="I28" s="41"/>
+      <c r="J28" s="41"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="37" t="n">
+      <c r="B29" s="36" t="n">
         <v>18</v>
       </c>
-      <c r="C29" s="37" t="s">
+      <c r="C29" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="D29" s="37" t="s">
+      <c r="D29" s="36" t="s">
         <v>154</v>
       </c>
-      <c r="E29" s="37" t="s">
+      <c r="E29" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="F29" s="37" t="n">
+      <c r="F29" s="36" t="n">
         <v>1</v>
       </c>
-      <c r="G29" s="37" t="n">
+      <c r="G29" s="36" t="n">
         <v>1</v>
       </c>
-      <c r="H29" s="37" t="s">
+      <c r="H29" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="I29" s="37"/>
-      <c r="J29" s="43" t="s">
+      <c r="I29" s="36"/>
+      <c r="J29" s="42" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="22" t="n">
+      <c r="B30" s="21" t="n">
         <v>19</v>
       </c>
-      <c r="C30" s="22" t="s">
+      <c r="C30" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="D30" s="44" t="s">
+      <c r="D30" s="43" t="s">
         <v>184</v>
       </c>
-      <c r="E30" s="44"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="22"/>
-      <c r="J30" s="24"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="23"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="26" t="n">
+      <c r="B31" s="25" t="n">
         <v>20</v>
       </c>
-      <c r="C31" s="45" t="s">
+      <c r="C31" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="D31" s="46" t="s">
+      <c r="D31" s="45" t="s">
         <v>185</v>
       </c>
-      <c r="E31" s="46" t="s">
+      <c r="E31" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="F31" s="46" t="n">
+      <c r="F31" s="45" t="n">
         <v>1</v>
       </c>
-      <c r="G31" s="47" t="s">
+      <c r="G31" s="46" t="s">
         <v>186</v>
       </c>
-      <c r="H31" s="46" t="s">
+      <c r="H31" s="45" t="s">
         <v>187</v>
       </c>
-      <c r="I31" s="26"/>
-      <c r="J31" s="20"/>
+      <c r="I31" s="25"/>
+      <c r="J31" s="19"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I32" s="1" t="s">
+      <c r="I32" s="0" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I33" s="1" t="s">
+      <c r="I33" s="0" t="s">
         <v>189</v>
       </c>
     </row>
@@ -3543,7 +3434,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3553,270 +3444,270 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="48" width="40.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="49" width="33.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="48" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="49" width="100.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="47" width="40.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="48" width="33.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="47" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="48" width="100.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="49" t="s">
         <v>190</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="52"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="51"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="52" t="s">
         <v>193</v>
       </c>
-      <c r="C8" s="54" t="s">
+      <c r="C8" s="53" t="s">
         <v>194</v>
       </c>
-      <c r="D8" s="53" t="s">
+      <c r="D8" s="52" t="s">
         <v>195</v>
       </c>
-      <c r="E8" s="54" t="s">
+      <c r="E8" s="53" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="54" t="s">
         <v>197</v>
       </c>
-      <c r="C9" s="56" t="s">
+      <c r="C9" s="55" t="s">
         <v>198</v>
       </c>
-      <c r="D9" s="57" t="n">
+      <c r="D9" s="56" t="n">
         <v>20</v>
       </c>
-      <c r="E9" s="58" t="s">
+      <c r="E9" s="57" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="55"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="56" t="s">
+      <c r="B10" s="54"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="55" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="55"/>
-      <c r="C11" s="56"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="56" t="s">
+      <c r="B11" s="54"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="55" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="55"/>
-      <c r="C12" s="59" t="s">
+      <c r="B12" s="54"/>
+      <c r="C12" s="58" t="s">
         <v>202</v>
       </c>
-      <c r="D12" s="60" t="n">
+      <c r="D12" s="59" t="n">
         <v>20</v>
       </c>
-      <c r="E12" s="61" t="s">
+      <c r="E12" s="60" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="55"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="61" t="s">
+      <c r="B13" s="54"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="60" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="55"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="60"/>
-      <c r="E14" s="59" t="s">
+      <c r="B14" s="54"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="58" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="55"/>
-      <c r="C15" s="62" t="s">
+      <c r="B15" s="54"/>
+      <c r="C15" s="61" t="s">
         <v>206</v>
       </c>
-      <c r="D15" s="57" t="n">
+      <c r="D15" s="56" t="n">
         <v>20</v>
       </c>
-      <c r="E15" s="58" t="s">
+      <c r="E15" s="57" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="55"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="63" t="s">
+      <c r="B16" s="54"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="62" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="55"/>
-      <c r="C17" s="62"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="63" t="s">
+      <c r="B17" s="54"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="62" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="55"/>
-      <c r="C18" s="62"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="63" t="s">
+      <c r="B18" s="54"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="62" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="55"/>
-      <c r="C19" s="64" t="s">
+      <c r="B19" s="54"/>
+      <c r="C19" s="63" t="s">
         <v>211</v>
       </c>
-      <c r="D19" s="60" t="n">
+      <c r="D19" s="59" t="n">
         <v>20</v>
       </c>
-      <c r="E19" s="61" t="s">
+      <c r="E19" s="60" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="55"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="61" t="s">
+      <c r="B20" s="54"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="60" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="55"/>
-      <c r="C21" s="64"/>
-      <c r="D21" s="60"/>
-      <c r="E21" s="61"/>
+      <c r="B21" s="54"/>
+      <c r="C21" s="63"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="60"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="55"/>
-      <c r="C22" s="65" t="s">
+      <c r="B22" s="54"/>
+      <c r="C22" s="64" t="s">
         <v>214</v>
       </c>
-      <c r="D22" s="57" t="n">
+      <c r="D22" s="56" t="n">
         <v>20</v>
       </c>
-      <c r="E22" s="58" t="s">
+      <c r="E22" s="57" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="55"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="58" t="s">
+      <c r="B23" s="54"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="57" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="66" t="s">
+      <c r="B25" s="65" t="s">
         <v>217</v>
       </c>
-      <c r="C25" s="67"/>
-      <c r="D25" s="68" t="n">
+      <c r="C25" s="66"/>
+      <c r="D25" s="67" t="n">
         <f aca="false">SUM(D9:D24)</f>
         <v>100</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="54" t="s">
+      <c r="C27" s="53" t="s">
         <v>218</v>
       </c>
-      <c r="D27" s="53" t="s">
+      <c r="D27" s="52" t="s">
         <v>195</v>
       </c>
-      <c r="E27" s="54" t="s">
+      <c r="E27" s="53" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C28" s="65" t="s">
+      <c r="C28" s="64" t="s">
         <v>219</v>
       </c>
-      <c r="D28" s="57" t="n">
+      <c r="D28" s="56" t="n">
         <v>100</v>
       </c>
-      <c r="E28" s="58" t="s">
+      <c r="E28" s="57" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="65"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="63" t="s">
+      <c r="C29" s="64"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="62" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="65"/>
-      <c r="D30" s="57"/>
-      <c r="E30" s="63" t="s">
+      <c r="C30" s="64"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="62" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="65"/>
-      <c r="D31" s="57"/>
-      <c r="E31" s="63" t="s">
+      <c r="C31" s="64"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="62" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="65"/>
-      <c r="D32" s="57"/>
-      <c r="E32" s="63" t="s">
+      <c r="C32" s="64"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="62" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D33" s="69"/>
+      <c r="D33" s="68"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D34" s="69"/>
+      <c r="D34" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3842,7 +3733,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3852,393 +3743,393 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="1.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="70.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="101.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="70.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="101.85"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="69" t="s">
         <v>225</v>
       </c>
-      <c r="F2" s="71" t="s">
+      <c r="F2" s="70" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F3" s="71" t="s">
+      <c r="F3" s="70" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="54" t="s">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="53" t="s">
         <v>194</v>
       </c>
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="52" t="s">
         <v>195</v>
       </c>
-      <c r="D4" s="72" t="s">
+      <c r="D4" s="71" t="s">
         <v>228</v>
       </c>
-      <c r="E4" s="54" t="s">
+      <c r="E4" s="53" t="s">
         <v>229</v>
       </c>
-      <c r="F4" s="54" t="s">
+      <c r="F4" s="53" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="72" t="s">
         <v>198</v>
       </c>
-      <c r="C5" s="57" t="n">
+      <c r="C5" s="56" t="n">
         <v>20</v>
       </c>
-      <c r="D5" s="57" t="n">
+      <c r="D5" s="56" t="n">
         <v>7</v>
       </c>
-      <c r="E5" s="58" t="s">
+      <c r="E5" s="57" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="73"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="56" t="s">
+      <c r="B6" s="72"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="55" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="73"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="56" t="s">
+      <c r="B7" s="72"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="55" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="74" t="s">
+      <c r="B8" s="73" t="s">
         <v>202</v>
       </c>
-      <c r="C8" s="60" t="n">
+      <c r="C8" s="59" t="n">
         <v>20</v>
       </c>
-      <c r="D8" s="60" t="n">
+      <c r="D8" s="59" t="n">
         <v>7</v>
       </c>
-      <c r="E8" s="61" t="s">
+      <c r="E8" s="60" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="74"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="61" t="s">
+      <c r="B9" s="73"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="60" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="74"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="59" t="s">
+      <c r="B10" s="73"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="58" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="75" t="s">
+      <c r="B11" s="74" t="s">
         <v>206</v>
       </c>
-      <c r="C11" s="57" t="n">
+      <c r="C11" s="56" t="n">
         <v>20</v>
       </c>
-      <c r="D11" s="76" t="n">
+      <c r="D11" s="75" t="n">
         <v>7</v>
       </c>
-      <c r="E11" s="58" t="s">
+      <c r="E11" s="57" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="75"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="63" t="s">
+      <c r="B12" s="74"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="62" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="75"/>
-      <c r="C13" s="57"/>
-      <c r="D13" s="76"/>
-      <c r="E13" s="63" t="s">
+      <c r="B13" s="74"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="75"/>
+      <c r="E13" s="62" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="75"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="76"/>
-      <c r="E14" s="63" t="s">
+      <c r="B14" s="74"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="75"/>
+      <c r="E14" s="62" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="77" t="s">
+      <c r="B15" s="76" t="s">
         <v>231</v>
       </c>
-      <c r="C15" s="60" t="n">
+      <c r="C15" s="59" t="n">
         <v>20</v>
       </c>
-      <c r="D15" s="78" t="n">
+      <c r="D15" s="77" t="n">
         <v>7</v>
       </c>
-      <c r="E15" s="61" t="s">
+      <c r="E15" s="60" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="77"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="61" t="s">
+      <c r="B16" s="76"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="77"/>
+      <c r="E16" s="60" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="79" t="s">
+      <c r="B17" s="78" t="s">
         <v>232</v>
       </c>
-      <c r="C17" s="57" t="n">
+      <c r="C17" s="56" t="n">
         <v>20</v>
       </c>
-      <c r="D17" s="80" t="n">
+      <c r="D17" s="79" t="n">
         <v>7</v>
       </c>
-      <c r="E17" s="58" t="s">
+      <c r="E17" s="57" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="79"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="80"/>
-      <c r="E18" s="58" t="s">
+      <c r="B18" s="78"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="79"/>
+      <c r="E18" s="57" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="81" t="s">
+      <c r="B19" s="80" t="s">
         <v>235</v>
       </c>
-      <c r="C19" s="81"/>
-      <c r="D19" s="81"/>
-      <c r="E19" s="81"/>
-    </row>
-    <row r="20" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="82" t="n">
+      <c r="C19" s="80"/>
+      <c r="D19" s="80"/>
+      <c r="E19" s="80"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="81" t="n">
         <f aca="false">SUM(C5:C18)</f>
         <v>100</v>
       </c>
-      <c r="D20" s="83" t="n">
+      <c r="D20" s="82" t="n">
         <f aca="false">(D5*C5+D8*C8+D11*C11+D15*C15+D17*C17)/C20</f>
         <v>7</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="70" t="s">
+      <c r="B22" s="69" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="54" t="s">
+      <c r="B24" s="53" t="s">
         <v>237</v>
       </c>
-      <c r="C24" s="53" t="s">
+      <c r="C24" s="52" t="s">
         <v>238</v>
       </c>
-      <c r="D24" s="84" t="s">
+      <c r="D24" s="83" t="s">
         <v>239</v>
       </c>
-      <c r="E24" s="54" t="s">
+      <c r="E24" s="53" t="s">
         <v>240</v>
       </c>
-      <c r="F24" s="54" t="s">
+      <c r="F24" s="53" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="0" t="s">
         <v>242</v>
       </c>
-      <c r="C25" s="1" t="n">
+      <c r="C25" s="0" t="n">
         <v>123456</v>
       </c>
-      <c r="D25" s="1" t="n">
+      <c r="D25" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="E25" s="85" t="n">
+      <c r="E25" s="84" t="n">
         <f aca="false">$D$20*D25/$D$34</f>
         <v>7</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F25" s="0" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="0" t="s">
         <v>242</v>
       </c>
-      <c r="C26" s="1" t="n">
+      <c r="C26" s="0" t="n">
         <v>123456</v>
       </c>
-      <c r="D26" s="1" t="n">
+      <c r="D26" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="E26" s="85" t="n">
+      <c r="E26" s="84" t="n">
         <f aca="false">$D$20*D26/$D$34</f>
         <v>7</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26" s="0" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="0" t="s">
         <v>242</v>
       </c>
-      <c r="C27" s="1" t="n">
+      <c r="C27" s="0" t="n">
         <v>123456</v>
       </c>
-      <c r="D27" s="1" t="n">
+      <c r="D27" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="E27" s="85" t="n">
+      <c r="E27" s="84" t="n">
         <f aca="false">$D$20*D27/$D$34</f>
         <v>7</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F27" s="0" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="0" t="s">
         <v>242</v>
       </c>
-      <c r="C28" s="1" t="n">
+      <c r="C28" s="0" t="n">
         <v>123456</v>
       </c>
-      <c r="D28" s="1" t="n">
+      <c r="D28" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="E28" s="85" t="n">
+      <c r="E28" s="84" t="n">
         <f aca="false">$D$20*D28/$D$34</f>
         <v>7</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F28" s="0" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="0" t="s">
         <v>242</v>
       </c>
-      <c r="C29" s="1" t="n">
+      <c r="C29" s="0" t="n">
         <v>123456</v>
       </c>
-      <c r="D29" s="1" t="n">
+      <c r="D29" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="E29" s="85" t="n">
+      <c r="E29" s="84" t="n">
         <f aca="false">$D$20*D29/$D$34</f>
         <v>7</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F29" s="0" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="0" t="s">
         <v>242</v>
       </c>
-      <c r="C30" s="1" t="n">
+      <c r="C30" s="0" t="n">
         <v>123456</v>
       </c>
-      <c r="D30" s="1" t="n">
+      <c r="D30" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="E30" s="85" t="n">
+      <c r="E30" s="84" t="n">
         <f aca="false">$D$20*D30/$D$34</f>
         <v>7</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F30" s="0" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="0" t="s">
         <v>242</v>
       </c>
-      <c r="C31" s="1" t="n">
+      <c r="C31" s="0" t="n">
         <v>123456</v>
       </c>
-      <c r="D31" s="1" t="n">
+      <c r="D31" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="E31" s="85" t="n">
+      <c r="E31" s="84" t="n">
         <f aca="false">$D$20*D31/$D$34</f>
         <v>7</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F31" s="0" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="0" t="s">
         <v>242</v>
       </c>
-      <c r="C32" s="1" t="n">
+      <c r="C32" s="0" t="n">
         <v>123456</v>
       </c>
-      <c r="D32" s="1" t="n">
+      <c r="D32" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="E32" s="85" t="n">
+      <c r="E32" s="84" t="n">
         <f aca="false">$D$20*D32/$D$34</f>
         <v>7</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="F32" s="0" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="86" t="s">
+      <c r="C34" s="85" t="s">
         <v>244</v>
       </c>
-      <c r="D34" s="1" t="n">
+      <c r="D34" s="0" t="n">
         <f aca="false">AVERAGE(D25:D32)</f>
         <v>7</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="0" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="0" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="0" t="s">
         <v>247</v>
       </c>
     </row>
@@ -4272,620 +4163,620 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="B2:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E53" activeCellId="0" sqref="E53"/>
+      <selection pane="topLeft" activeCell="E42" activeCellId="0" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="1.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="70.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="101.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="70.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="101.85"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="69" t="s">
         <v>248</v>
       </c>
-      <c r="F2" s="71" t="s">
+      <c r="F2" s="70" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F3" s="71" t="s">
+      <c r="F3" s="70" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="54" t="s">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="53" t="s">
         <v>194</v>
       </c>
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="52" t="s">
         <v>195</v>
       </c>
-      <c r="D4" s="72" t="s">
+      <c r="D4" s="71" t="s">
         <v>249</v>
       </c>
-      <c r="E4" s="54" t="s">
+      <c r="E4" s="53" t="s">
         <v>229</v>
       </c>
-      <c r="F4" s="54" t="s">
+      <c r="F4" s="53" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="72" t="s">
         <v>198</v>
       </c>
-      <c r="C5" s="57" t="n">
+      <c r="C5" s="56" t="n">
         <v>20</v>
       </c>
-      <c r="D5" s="80" t="n">
-        <v>9</v>
-      </c>
-      <c r="E5" s="58" t="s">
+      <c r="D5" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="57" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="73"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="80"/>
-      <c r="E6" s="56" t="s">
+      <c r="B6" s="72"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="79"/>
+      <c r="E6" s="55" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="73"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="80"/>
-      <c r="E7" s="56" t="s">
+      <c r="B7" s="72"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="55" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="74" t="s">
+      <c r="B8" s="73" t="s">
         <v>202</v>
       </c>
-      <c r="C8" s="60" t="n">
+      <c r="C8" s="59" t="n">
         <v>20</v>
       </c>
-      <c r="D8" s="78" t="n">
-        <v>9</v>
-      </c>
-      <c r="E8" s="61" t="s">
+      <c r="D8" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="60" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="74"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="61" t="s">
+      <c r="B9" s="73"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="77"/>
+      <c r="E9" s="60" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="74"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="78"/>
-      <c r="E10" s="59" t="s">
+      <c r="B10" s="73"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="77"/>
+      <c r="E10" s="58" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="75" t="s">
+      <c r="B11" s="74" t="s">
         <v>206</v>
       </c>
-      <c r="C11" s="57" t="n">
+      <c r="C11" s="56" t="n">
         <v>20</v>
       </c>
-      <c r="D11" s="87" t="n">
-        <v>9</v>
-      </c>
-      <c r="E11" s="58" t="s">
+      <c r="D11" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="57" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="75"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="87"/>
-      <c r="E12" s="63" t="s">
+      <c r="B12" s="74"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="62" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="75"/>
-      <c r="C13" s="57"/>
-      <c r="D13" s="87"/>
-      <c r="E13" s="63" t="s">
+      <c r="B13" s="74"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="86"/>
+      <c r="E13" s="62" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="75"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="87"/>
-      <c r="E14" s="63" t="s">
+      <c r="B14" s="74"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="86"/>
+      <c r="E14" s="62" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="77" t="s">
+      <c r="B15" s="76" t="s">
         <v>231</v>
       </c>
-      <c r="C15" s="60" t="n">
+      <c r="C15" s="59" t="n">
         <v>20</v>
       </c>
-      <c r="D15" s="78" t="n">
-        <v>10</v>
-      </c>
-      <c r="E15" s="61" t="s">
+      <c r="D15" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="60" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="77"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="61" t="s">
+      <c r="B16" s="76"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="77"/>
+      <c r="E16" s="60" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="79" t="s">
+      <c r="B17" s="78" t="s">
         <v>232</v>
       </c>
-      <c r="C17" s="57" t="n">
+      <c r="C17" s="56" t="n">
         <v>20</v>
       </c>
-      <c r="D17" s="80" t="n">
-        <v>9</v>
-      </c>
-      <c r="E17" s="58" t="s">
+      <c r="D17" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="57" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="79"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="80"/>
-      <c r="E18" s="58" t="s">
+    <row r="18" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="78"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="79"/>
+      <c r="E18" s="57" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="81" t="s">
+      <c r="B19" s="80" t="s">
         <v>251</v>
       </c>
-      <c r="C19" s="81"/>
-      <c r="D19" s="81"/>
-      <c r="E19" s="81"/>
-    </row>
-    <row r="20" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="82" t="n">
+      <c r="C19" s="80"/>
+      <c r="D19" s="80"/>
+      <c r="E19" s="80"/>
+    </row>
+    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="81" t="n">
         <f aca="false">SUM(C5:C18)</f>
         <v>100</v>
       </c>
-      <c r="D20" s="83" t="n">
+      <c r="D20" s="82" t="n">
         <f aca="false">(D5*C5+D8*C8+D11*C11+D15*C15+D17*C17)/C20</f>
-        <v>9.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="71" t="s">
+      <c r="B22" s="70" t="s">
         <v>252</v>
       </c>
-      <c r="F22" s="88" t="s">
+      <c r="F22" s="87" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="71" t="s">
+      <c r="B23" s="70" t="s">
         <v>254</v>
       </c>
-      <c r="F23" s="89"/>
+      <c r="F23" s="88"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F24" s="89"/>
+      <c r="F24" s="88"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C25" s="90" t="s">
+      <c r="C25" s="89" t="s">
         <v>255</v>
       </c>
-      <c r="D25" s="90"/>
-      <c r="F25" s="89"/>
-    </row>
-    <row r="26" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="91" t="s">
+      <c r="D25" s="89"/>
+      <c r="F25" s="88"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="90" t="s">
         <v>256</v>
       </c>
-      <c r="C26" s="90" t="s">
+      <c r="C26" s="89" t="s">
         <v>257</v>
       </c>
-      <c r="D26" s="90" t="s">
+      <c r="D26" s="89" t="s">
         <v>258</v>
       </c>
-      <c r="E26" s="92" t="s">
+      <c r="E26" s="91" t="s">
         <v>259</v>
       </c>
-      <c r="F26" s="89"/>
+      <c r="F26" s="88"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="1" t="n">
+      <c r="B27" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="F27" s="89"/>
+      <c r="F27" s="88"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="1" t="n">
+      <c r="B28" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="F28" s="89"/>
+      <c r="F28" s="88"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="1" t="n">
+      <c r="B29" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="89"/>
+      <c r="F29" s="88"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="1" t="n">
+      <c r="B30" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="F30" s="89"/>
+      <c r="F30" s="88"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="1" t="n">
+      <c r="B31" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="F31" s="89"/>
+      <c r="F31" s="88"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="1" t="n">
+      <c r="B32" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="F32" s="89"/>
+      <c r="F32" s="88"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="1" t="n">
+      <c r="B33" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="F33" s="89"/>
+      <c r="F33" s="88"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="1" t="n">
+      <c r="B34" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="F34" s="89"/>
+      <c r="F34" s="88"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="1" t="n">
+      <c r="B35" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="F35" s="89"/>
+      <c r="F35" s="88"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="1" t="n">
+      <c r="B36" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="F36" s="89"/>
+      <c r="F36" s="88"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="1" t="n">
+      <c r="B37" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="F37" s="89"/>
+      <c r="F37" s="88"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="1" t="n">
+      <c r="B38" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="F38" s="89"/>
+      <c r="F38" s="88"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="1" t="n">
+      <c r="B39" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="F39" s="89"/>
+      <c r="F39" s="88"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="1" t="n">
+      <c r="B40" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="F40" s="89"/>
+      <c r="F40" s="88"/>
     </row>
     <row r="41" customFormat="false" ht="5.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B41" s="93"/>
-      <c r="C41" s="93"/>
-      <c r="D41" s="93"/>
-      <c r="E41" s="93"/>
-      <c r="F41" s="89"/>
+      <c r="B41" s="92"/>
+      <c r="C41" s="92"/>
+      <c r="D41" s="92"/>
+      <c r="E41" s="92"/>
+      <c r="F41" s="88"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="1" t="n">
+      <c r="B42" s="0" t="n">
         <v>101</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" s="0" t="s">
         <v>262</v>
       </c>
-      <c r="F42" s="89"/>
+      <c r="F42" s="88"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="1" t="n">
+      <c r="B43" s="0" t="n">
         <v>102</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E43" s="0" t="s">
         <v>264</v>
       </c>
-      <c r="F43" s="89"/>
+      <c r="F43" s="88"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="1" t="n">
+      <c r="B44" s="0" t="n">
         <v>103</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E44" s="0" t="s">
         <v>265</v>
       </c>
-      <c r="F44" s="89"/>
+      <c r="F44" s="88"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="1" t="n">
+      <c r="B45" s="0" t="n">
         <v>104</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E45" s="0" t="s">
         <v>266</v>
       </c>
-      <c r="F45" s="89"/>
+      <c r="F45" s="88"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="1" t="n">
+      <c r="B46" s="0" t="n">
         <v>105</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E46" s="0" t="s">
         <v>267</v>
       </c>
-      <c r="F46" s="89"/>
+      <c r="F46" s="88"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="1" t="n">
+      <c r="B47" s="0" t="n">
         <v>106</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E47" s="0" t="s">
         <v>268</v>
       </c>
-      <c r="F47" s="89"/>
+      <c r="F47" s="88"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="70" t="s">
+      <c r="B49" s="69" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="54" t="s">
+      <c r="B51" s="53" t="s">
         <v>237</v>
       </c>
-      <c r="C51" s="53" t="s">
+      <c r="C51" s="52" t="s">
         <v>238</v>
       </c>
-      <c r="D51" s="84" t="s">
+      <c r="D51" s="83" t="s">
         <v>239</v>
       </c>
-      <c r="E51" s="54" t="s">
+      <c r="E51" s="53" t="s">
         <v>270</v>
       </c>
-      <c r="F51" s="54" t="s">
+      <c r="F51" s="53" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="1" t="s">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="0" t="s">
         <v>271</v>
       </c>
-      <c r="C52" s="1" t="n">
+      <c r="C52" s="0" t="n">
         <v>2183499</v>
       </c>
-      <c r="D52" s="1" t="n">
+      <c r="D52" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="E52" s="85" t="n">
+      <c r="E52" s="84" t="n">
         <f aca="false">$D$20*D52/$D$58</f>
-        <v>10.0821917808219</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="0" t="s">
         <v>272</v>
       </c>
-      <c r="C53" s="1" t="n">
+      <c r="C53" s="0" t="n">
         <v>2184122</v>
       </c>
-      <c r="D53" s="1" t="n">
+      <c r="D53" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="E53" s="85" t="n">
+      <c r="E53" s="84" t="n">
         <f aca="false">$D$20*D53/$D$58</f>
-        <v>10.0821917808219</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="0" t="s">
         <v>273</v>
       </c>
-      <c r="C54" s="1" t="n">
+      <c r="C54" s="0" t="n">
         <v>2184441</v>
       </c>
-      <c r="D54" s="1" t="n">
+      <c r="D54" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="E54" s="85" t="n">
+      <c r="E54" s="84" t="n">
         <f aca="false">$D$20*D54/$D$58</f>
-        <v>10.0821917808219</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="0" t="s">
         <v>274</v>
       </c>
-      <c r="C55" s="1" t="n">
+      <c r="C55" s="0" t="n">
         <v>2177643</v>
       </c>
-      <c r="D55" s="1" t="n">
+      <c r="D55" s="0" t="n">
         <v>6.5</v>
       </c>
-      <c r="E55" s="85" t="n">
+      <c r="E55" s="84" t="n">
         <f aca="false">$D$20*D55/$D$58</f>
-        <v>8.19178082191781</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="0" t="s">
         <v>275</v>
       </c>
-      <c r="C56" s="1" t="n">
+      <c r="C56" s="0" t="n">
         <v>2154689</v>
       </c>
-      <c r="D56" s="1" t="n">
+      <c r="D56" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="E56" s="85" t="n">
+      <c r="E56" s="84" t="n">
         <f aca="false">$D$20*D56/$D$58</f>
-        <v>7.56164383561644</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C58" s="86" t="s">
+      <c r="C58" s="85" t="s">
         <v>244</v>
       </c>
-      <c r="D58" s="1" t="n">
+      <c r="D58" s="0" t="n">
         <f aca="false">AVERAGE(D52:D56)</f>
         <v>7.3</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="1" t="s">
+      <c r="B60" s="0" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="0" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="1" t="s">
+      <c r="B62" s="0" t="s">
         <v>247</v>
       </c>
     </row>
@@ -4924,7 +4815,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -4934,54 +4825,54 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="122.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="122.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="0" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="94" t="s">
+      <c r="B2" s="93" t="s">
         <v>277</v>
       </c>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
     </row>
     <row r="3" customFormat="false" ht="5.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="70" t="s">
+      <c r="B4" s="69" t="s">
         <v>278</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="C4" s="69" t="s">
         <v>279</v>
       </c>
-      <c r="D4" s="70" t="s">
+      <c r="D4" s="69" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="95" t="n">
+      <c r="B5" s="94" t="n">
         <v>45527</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="96" t="s">
+      <c r="D5" s="95" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="97"/>
-      <c r="C7" s="86"/>
+      <c r="B7" s="96"/>
+      <c r="C7" s="85"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="95"/>
+      <c r="B8" s="94"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Revert "Revert "merging documents into development to remove unnecessary files""
</commit_message>
<xml_diff>
--- a/docs/assessment/handin/papierwerk.xlsx
+++ b/docs/assessment/handin/papierwerk.xlsx
@@ -8,13 +8,13 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="Opdracht" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Userstories" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Planning" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Toetsmatrijs" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Beoordeling P1" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Beoordeling P2" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Versiebeheer" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Opdracht" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Userstories" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Planning" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Toetsmatrijs" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="Beoordeling P1" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="Beoordeling P2" sheetId="6" state="visible" r:id="rId8"/>
+    <sheet name="Versiebeheer" sheetId="7" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -959,11 +959,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
   </numFmts>
   <fonts count="19">
     <font>
@@ -1317,392 +1316,396 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="17" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="17" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="15" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="15" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="16" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="18" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="18" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="17" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="17" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="14" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="14" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1778,8 +1781,114 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1789,114 +1898,114 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="113.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="113.85"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="3"/>
+      <c r="C8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="335.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="7" t="s">
+    <row r="13" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="7"/>
-      <c r="C14" s="8" t="s">
+      <c r="B14" s="8"/>
+      <c r="C14" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="7"/>
-      <c r="C15" s="8" t="s">
+      <c r="B15" s="8"/>
+      <c r="C15" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="7"/>
-      <c r="C16" s="8" t="s">
+      <c r="B16" s="8"/>
+      <c r="C16" s="9" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="9"/>
-      <c r="C18" s="10" t="s">
+      <c r="B18" s="10"/>
+      <c r="C18" s="11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="6"/>
-      <c r="C19" s="6" t="s">
+      <c r="B19" s="7"/>
+      <c r="C19" s="7" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1915,7 +2024,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1925,681 +2034,681 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="136.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="1.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="136.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="4"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="12"/>
+      <c r="C3" s="13"/>
     </row>
     <row r="4" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="66" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="13"/>
+      <c r="C10" s="14"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="13"/>
+      <c r="C15" s="14"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="13"/>
+      <c r="C20" s="14"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="13"/>
+      <c r="C25" s="14"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="13"/>
+      <c r="C30" s="14"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="C33" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C35" s="13"/>
+      <c r="C35" s="14"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="C36" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="C37" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C38" s="0" t="s">
+      <c r="C38" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="13" t="s">
+      <c r="B40" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C40" s="13"/>
+      <c r="C40" s="14"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="0" t="s">
+      <c r="B41" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C41" s="0" t="s">
+      <c r="C41" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="0" t="s">
+      <c r="B42" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C42" s="0" t="s">
+      <c r="C42" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="0" t="s">
+      <c r="B43" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="C43" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="13" t="s">
+      <c r="B45" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C45" s="13"/>
+      <c r="C45" s="14"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="0" t="s">
+      <c r="B46" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="C46" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0" t="s">
+      <c r="B47" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C47" s="0" t="s">
+      <c r="C47" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="0" t="s">
+      <c r="B48" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C48" s="0" t="s">
+      <c r="C48" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="13" t="s">
+      <c r="B50" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C50" s="13"/>
+      <c r="C50" s="14"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="0" t="s">
+      <c r="B51" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C51" s="0" t="s">
+      <c r="C51" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="0" t="s">
+      <c r="B52" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C52" s="0" t="s">
+      <c r="C52" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="0" t="s">
+      <c r="B53" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C53" s="0" t="s">
+      <c r="C53" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="13" t="s">
+      <c r="B55" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C55" s="13"/>
+      <c r="C55" s="14"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="0" t="s">
+      <c r="B56" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C56" s="0" t="s">
+      <c r="C56" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="0" t="s">
+      <c r="B57" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C57" s="0" t="s">
+      <c r="C57" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="0" t="s">
+      <c r="B58" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C58" s="0" t="s">
+      <c r="C58" s="1" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="13" t="s">
+      <c r="B60" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="C60" s="13"/>
+      <c r="C60" s="14"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="0" t="s">
+      <c r="B61" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C61" s="0" t="s">
+      <c r="C61" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="0" t="s">
+      <c r="B62" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C62" s="0" t="s">
+      <c r="C62" s="1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="0" t="s">
+      <c r="B63" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C63" s="0" t="s">
+      <c r="C63" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="13" t="s">
+      <c r="B65" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="C65" s="13"/>
+      <c r="C65" s="14"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="0" t="s">
+      <c r="B66" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C66" s="0" t="s">
+      <c r="C66" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="0" t="s">
+      <c r="B67" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C67" s="0" t="s">
+      <c r="C67" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="0" t="s">
+      <c r="B68" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C68" s="0" t="s">
+      <c r="C68" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="13" t="s">
+      <c r="B70" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C70" s="13"/>
+      <c r="C70" s="14"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="0" t="s">
+      <c r="B71" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C71" s="0" t="s">
+      <c r="C71" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="0" t="s">
+      <c r="B72" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C72" s="0" t="s">
+      <c r="C72" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="0" t="s">
+      <c r="B73" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C73" s="0" t="s">
+      <c r="C73" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="13" t="s">
+      <c r="B75" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="C75" s="13"/>
+      <c r="C75" s="14"/>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="0" t="s">
+      <c r="B76" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C76" s="0" t="s">
+      <c r="C76" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="0" t="s">
+      <c r="B77" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C77" s="0" t="s">
+      <c r="C77" s="1" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="0" t="s">
+      <c r="B78" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C78" s="0" t="s">
+      <c r="C78" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="14" t="s">
+      <c r="A80" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="B80" s="14"/>
-      <c r="C80" s="14"/>
-      <c r="D80" s="14"/>
+      <c r="B80" s="15"/>
+      <c r="C80" s="15"/>
+      <c r="D80" s="15"/>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D81" s="15" t="s">
+      <c r="D81" s="16" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="13" t="s">
+      <c r="B82" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C82" s="16"/>
-      <c r="D82" s="17" t="n">
+      <c r="C82" s="17"/>
+      <c r="D82" s="18" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="0" t="s">
+      <c r="B83" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C83" s="0" t="s">
+      <c r="C83" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="0" t="s">
+      <c r="B84" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C84" s="0" t="s">
+      <c r="C84" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B85" s="0" t="s">
+      <c r="B85" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C85" s="0" t="s">
+      <c r="C85" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B87" s="13" t="s">
+      <c r="B87" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="C87" s="16"/>
-      <c r="D87" s="17" t="n">
+      <c r="C87" s="17"/>
+      <c r="D87" s="18" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B88" s="0" t="s">
+      <c r="B88" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C88" s="0" t="s">
+      <c r="C88" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B89" s="0" t="s">
+      <c r="B89" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C89" s="0" t="s">
+      <c r="C89" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B90" s="0" t="s">
+      <c r="B90" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C90" s="0" t="s">
+      <c r="C90" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B92" s="13" t="s">
+      <c r="B92" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="C92" s="16"/>
-      <c r="D92" s="17" t="n">
+      <c r="C92" s="17"/>
+      <c r="D92" s="18" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B93" s="0" t="s">
+      <c r="B93" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C93" s="0" t="s">
+      <c r="C93" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B94" s="0" t="s">
+      <c r="B94" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C94" s="0" t="s">
+      <c r="C94" s="1" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B95" s="0" t="s">
+      <c r="B95" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C95" s="0" t="s">
+      <c r="C95" s="1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B97" s="13" t="s">
+      <c r="B97" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="C97" s="16"/>
-      <c r="D97" s="17" t="n">
+      <c r="C97" s="17"/>
+      <c r="D97" s="18" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B98" s="0" t="s">
+      <c r="B98" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C98" s="0" t="s">
+      <c r="C98" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B99" s="0" t="s">
+      <c r="B99" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C99" s="0" t="s">
+      <c r="C99" s="1" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B100" s="0" t="s">
+      <c r="B100" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C100" s="0" t="s">
+      <c r="C100" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B102" s="13" t="s">
+      <c r="B102" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="C102" s="16"/>
-      <c r="D102" s="17" t="n">
+      <c r="C102" s="17"/>
+      <c r="D102" s="18" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B103" s="0" t="s">
+      <c r="B103" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C103" s="0" t="s">
+      <c r="C103" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B104" s="0" t="s">
+      <c r="B104" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C104" s="0" t="s">
+      <c r="C104" s="1" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B105" s="0" t="s">
+      <c r="B105" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C105" s="0" t="s">
+      <c r="C105" s="1" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B107" s="13" t="s">
+      <c r="B107" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="C107" s="16"/>
-      <c r="D107" s="17" t="n">
+      <c r="C107" s="17"/>
+      <c r="D107" s="18" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B108" s="0" t="s">
+      <c r="B108" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C108" s="0" t="s">
+      <c r="C108" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B109" s="0" t="s">
+      <c r="B109" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C109" s="0" t="s">
+      <c r="C109" s="1" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B110" s="0" t="s">
+      <c r="B110" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C110" s="0" t="s">
+      <c r="C110" s="1" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2623,7 +2732,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2633,787 +2742,787 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="1.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="74.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="1.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="1.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="6.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="5.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="6.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="25.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="74.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="77"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="4.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
     </row>
     <row r="4" customFormat="false" ht="3.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="I5" s="20" t="s">
+      <c r="I5" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="J5" s="20" t="s">
+      <c r="J5" s="21" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="21" t="n">
+      <c r="B6" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="G6" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="H6" s="21" t="s">
+      <c r="H6" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="I6" s="21" t="s">
+      <c r="I6" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="J6" s="23" t="s">
+      <c r="J6" s="24" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="F7" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="G7" s="21" t="n">
+      <c r="G7" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="I7" s="21" t="s">
+      <c r="I7" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="J7" s="23" t="s">
+      <c r="J7" s="24" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="24" t="n">
+      <c r="B8" s="25" t="n">
         <v>2</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="G8" s="24" t="n">
+      <c r="G8" s="25" t="n">
         <v>3</v>
       </c>
-      <c r="H8" s="24" t="s">
+      <c r="H8" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="I8" s="24" t="s">
+      <c r="I8" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="J8" s="26" t="s">
+      <c r="J8" s="27" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="21" t="n">
+      <c r="B9" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="G9" s="21" t="n">
+      <c r="G9" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="H9" s="21" t="s">
+      <c r="H9" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="I9" s="21" t="s">
+      <c r="I9" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="J9" s="23" t="s">
+      <c r="J9" s="24" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="28" t="n">
+      <c r="B10" s="29" t="n">
         <v>4</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="F10" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="G10" s="24" t="n">
+      <c r="G10" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="H10" s="24" t="s">
+      <c r="H10" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="I10" s="24" t="s">
+      <c r="I10" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="J10" s="26" t="s">
+      <c r="J10" s="27" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="21" t="n">
+      <c r="B11" s="22" t="n">
         <v>5</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="G11" s="21" t="n">
+      <c r="G11" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="H11" s="21" t="s">
+      <c r="H11" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="I11" s="21" t="s">
+      <c r="I11" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="J11" s="23" t="s">
+      <c r="J11" s="24" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="24" t="n">
+      <c r="B12" s="25" t="n">
         <v>6</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="F12" s="24" t="s">
+      <c r="F12" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="G12" s="24" t="n">
+      <c r="G12" s="25" t="n">
         <v>3</v>
       </c>
-      <c r="H12" s="24" t="s">
+      <c r="H12" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="I12" s="24" t="s">
+      <c r="I12" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="J12" s="26" t="s">
+      <c r="J12" s="27" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="21" t="n">
+      <c r="B13" s="22" t="n">
         <v>7</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="F13" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="G13" s="22" t="s">
+      <c r="G13" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="H13" s="21" t="s">
+      <c r="H13" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="I13" s="21" t="s">
+      <c r="I13" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="J13" s="23" t="s">
+      <c r="J13" s="24" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D14" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="F14" s="29" t="s">
+      <c r="F14" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="G14" s="30" t="s">
+      <c r="G14" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="H14" s="21" t="s">
+      <c r="H14" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="I14" s="21" t="s">
+      <c r="I14" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="J14" s="23" t="s">
+      <c r="J14" s="24" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="24" t="n">
+      <c r="B15" s="25" t="n">
         <v>8</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="E15" s="25"/>
-      <c r="F15" s="24" t="s">
+      <c r="E15" s="26"/>
+      <c r="F15" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="24" t="s">
+      <c r="G15" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="H15" s="24" t="s">
+      <c r="H15" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="I15" s="24" t="s">
+      <c r="I15" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="J15" s="26" t="s">
+      <c r="J15" s="27" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="21" t="n">
+      <c r="B16" s="22" t="n">
         <v>9</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="D16" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="E16" s="21"/>
-      <c r="F16" s="27" t="s">
+      <c r="E16" s="22"/>
+      <c r="F16" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="G16" s="27" t="s">
+      <c r="G16" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="H16" s="21" t="s">
+      <c r="H16" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="I16" s="21" t="s">
+      <c r="I16" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="J16" s="23" t="s">
+      <c r="J16" s="24" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="28" t="n">
+      <c r="B17" s="29" t="n">
         <v>10</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="D17" s="24" t="s">
+      <c r="D17" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="E17" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="F17" s="31" t="s">
+      <c r="F17" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="G17" s="24" t="n">
+      <c r="G17" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="H17" s="24" t="s">
+      <c r="H17" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="I17" s="24" t="s">
+      <c r="I17" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="J17" s="26" t="s">
+      <c r="J17" s="27" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="D18" s="32"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="24" t="s">
+      <c r="D18" s="33"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="G18" s="24" t="s">
+      <c r="G18" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="H18" s="24" t="s">
+      <c r="H18" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="I18" s="24" t="s">
+      <c r="I18" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="J18" s="26" t="s">
+      <c r="J18" s="27" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="33" t="n">
+      <c r="B19" s="34" t="n">
         <v>11</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="D19" s="33" t="s">
+      <c r="D19" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="E19" s="33" t="s">
+      <c r="E19" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="F19" s="33" t="n">
+      <c r="F19" s="34" t="n">
         <v>3</v>
       </c>
-      <c r="G19" s="33" t="n">
+      <c r="G19" s="34" t="n">
         <v>4</v>
       </c>
-      <c r="H19" s="33" t="s">
+      <c r="H19" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="I19" s="33" t="s">
+      <c r="I19" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="J19" s="34" t="s">
+      <c r="J19" s="35" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33" t="s">
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34" t="s">
         <v>154</v>
       </c>
-      <c r="E20" s="33" t="s">
+      <c r="E20" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="F20" s="33" t="s">
+      <c r="F20" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="G20" s="33" t="n">
+      <c r="G20" s="34" t="n">
         <v>1</v>
       </c>
-      <c r="H20" s="33" t="s">
+      <c r="H20" s="34" t="s">
         <v>156</v>
       </c>
-      <c r="I20" s="33" t="s">
+      <c r="I20" s="34" t="s">
         <v>157</v>
       </c>
-      <c r="J20" s="34" t="s">
+      <c r="J20" s="35" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="35" t="n">
+      <c r="B21" s="36" t="n">
         <v>12</v>
       </c>
-      <c r="C21" s="35" t="s">
+      <c r="C21" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="D21" s="35" t="s">
+      <c r="D21" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="E21" s="36" t="s">
+      <c r="E21" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="F21" s="35" t="n">
+      <c r="F21" s="36" t="n">
         <v>3</v>
       </c>
-      <c r="G21" s="35" t="n">
+      <c r="G21" s="36" t="n">
         <v>4</v>
       </c>
-      <c r="H21" s="35" t="s">
+      <c r="H21" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="I21" s="35" t="s">
+      <c r="I21" s="36" t="s">
         <v>160</v>
       </c>
-      <c r="J21" s="37" t="s">
+      <c r="J21" s="38" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="33" t="n">
+      <c r="B22" s="34" t="n">
         <v>13</v>
       </c>
-      <c r="C22" s="38" t="s">
+      <c r="C22" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="D22" s="33" t="s">
+      <c r="D22" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="E22" s="33" t="s">
+      <c r="E22" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="F22" s="33" t="n">
+      <c r="F22" s="34" t="n">
         <v>3</v>
       </c>
-      <c r="G22" s="33" t="n">
+      <c r="G22" s="34" t="n">
         <v>4</v>
       </c>
-      <c r="H22" s="33" t="s">
+      <c r="H22" s="34" t="s">
         <v>162</v>
       </c>
-      <c r="I22" s="33" t="s">
+      <c r="I22" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="J22" s="34" t="s">
+      <c r="J22" s="35" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="35" t="n">
+      <c r="B23" s="36" t="n">
         <v>14</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="D23" s="35" t="s">
+      <c r="D23" s="36" t="s">
         <v>165</v>
       </c>
-      <c r="E23" s="36" t="s">
+      <c r="E23" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="F23" s="39" t="s">
+      <c r="F23" s="40" t="s">
         <v>137</v>
       </c>
-      <c r="G23" s="39" t="s">
+      <c r="G23" s="40" t="s">
         <v>137</v>
       </c>
-      <c r="H23" s="35" t="s">
+      <c r="H23" s="36" t="s">
         <v>166</v>
       </c>
-      <c r="I23" s="35" t="s">
+      <c r="I23" s="36" t="s">
         <v>167</v>
       </c>
-      <c r="J23" s="37" t="s">
+      <c r="J23" s="38" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="33" t="n">
+      <c r="B24" s="34" t="n">
         <v>15</v>
       </c>
-      <c r="C24" s="33" t="s">
+      <c r="C24" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="D24" s="33" t="s">
+      <c r="D24" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="E24" s="33" t="s">
+      <c r="E24" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="F24" s="33" t="n">
+      <c r="F24" s="34" t="n">
         <v>3</v>
       </c>
-      <c r="G24" s="33" t="n">
+      <c r="G24" s="34" t="n">
         <v>4</v>
       </c>
-      <c r="H24" s="33" t="s">
+      <c r="H24" s="34" t="s">
         <v>169</v>
       </c>
-      <c r="I24" s="33" t="s">
+      <c r="I24" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="J24" s="34" t="s">
+      <c r="J24" s="35" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="35" t="n">
+      <c r="B25" s="36" t="n">
         <v>16</v>
       </c>
-      <c r="C25" s="35" t="s">
+      <c r="C25" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="D25" s="35" t="s">
+      <c r="D25" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="E25" s="36" t="s">
+      <c r="E25" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="F25" s="35" t="n">
+      <c r="F25" s="36" t="n">
         <v>1</v>
       </c>
-      <c r="G25" s="35" t="n">
+      <c r="G25" s="36" t="n">
         <v>1</v>
       </c>
-      <c r="H25" s="35" t="s">
+      <c r="H25" s="36" t="s">
         <v>172</v>
       </c>
-      <c r="I25" s="35" t="s">
+      <c r="I25" s="36" t="s">
         <v>173</v>
       </c>
-      <c r="J25" s="37" t="s">
+      <c r="J25" s="38" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="38" t="n">
+      <c r="B26" s="39" t="n">
         <v>17</v>
       </c>
-      <c r="C26" s="38" t="s">
+      <c r="C26" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="D26" s="33" t="s">
+      <c r="D26" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="E26" s="33" t="s">
+      <c r="E26" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="F26" s="33" t="n">
+      <c r="F26" s="34" t="n">
         <v>3</v>
       </c>
-      <c r="G26" s="40" t="s">
+      <c r="G26" s="41" t="s">
         <v>176</v>
       </c>
-      <c r="H26" s="33" t="s">
+      <c r="H26" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="I26" s="33" t="s">
+      <c r="I26" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="J26" s="34" t="s">
+      <c r="J26" s="35" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="33" t="s">
+      <c r="B27" s="39"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33" t="s">
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34" t="s">
         <v>180</v>
       </c>
-      <c r="I27" s="33"/>
-      <c r="J27" s="34" t="s">
+      <c r="I27" s="34"/>
+      <c r="J27" s="35" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="41" t="s">
+      <c r="B28" s="42" t="s">
         <v>182</v>
       </c>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="41"/>
-      <c r="I28" s="41"/>
-      <c r="J28" s="41"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="42"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="36" t="n">
+      <c r="B29" s="37" t="n">
         <v>18</v>
       </c>
-      <c r="C29" s="36" t="s">
+      <c r="C29" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="D29" s="36" t="s">
+      <c r="D29" s="37" t="s">
         <v>154</v>
       </c>
-      <c r="E29" s="36" t="s">
+      <c r="E29" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="F29" s="36" t="n">
+      <c r="F29" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="G29" s="36" t="n">
+      <c r="G29" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="H29" s="36" t="s">
+      <c r="H29" s="37" t="s">
         <v>180</v>
       </c>
-      <c r="I29" s="36"/>
-      <c r="J29" s="42" t="s">
+      <c r="I29" s="37"/>
+      <c r="J29" s="43" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="21" t="n">
+      <c r="B30" s="22" t="n">
         <v>19</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C30" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="D30" s="43" t="s">
+      <c r="D30" s="44" t="s">
         <v>184</v>
       </c>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="43"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="23"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="24"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="25" t="n">
+      <c r="B31" s="26" t="n">
         <v>20</v>
       </c>
-      <c r="C31" s="44" t="s">
+      <c r="C31" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="D31" s="45" t="s">
+      <c r="D31" s="46" t="s">
         <v>185</v>
       </c>
-      <c r="E31" s="45" t="s">
+      <c r="E31" s="46" t="s">
         <v>103</v>
       </c>
-      <c r="F31" s="45" t="n">
+      <c r="F31" s="46" t="n">
         <v>1</v>
       </c>
-      <c r="G31" s="46" t="s">
+      <c r="G31" s="47" t="s">
         <v>186</v>
       </c>
-      <c r="H31" s="45" t="s">
+      <c r="H31" s="46" t="s">
         <v>187</v>
       </c>
-      <c r="I31" s="25"/>
-      <c r="J31" s="19"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="20"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I32" s="0" t="s">
+      <c r="I32" s="1" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I33" s="0" t="s">
+      <c r="I33" s="1" t="s">
         <v>189</v>
       </c>
     </row>
@@ -3434,7 +3543,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3444,270 +3553,270 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="47" width="40.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="48" width="33.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="47" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="48" width="100.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="48" width="40.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="49" width="33.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="48" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="49" width="100.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="50" t="s">
         <v>190</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="52"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="53" t="s">
         <v>193</v>
       </c>
-      <c r="C8" s="53" t="s">
+      <c r="C8" s="54" t="s">
         <v>194</v>
       </c>
-      <c r="D8" s="52" t="s">
+      <c r="D8" s="53" t="s">
         <v>195</v>
       </c>
-      <c r="E8" s="53" t="s">
+      <c r="E8" s="54" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="54" t="s">
+      <c r="B9" s="55" t="s">
         <v>197</v>
       </c>
-      <c r="C9" s="55" t="s">
+      <c r="C9" s="56" t="s">
         <v>198</v>
       </c>
-      <c r="D9" s="56" t="n">
+      <c r="D9" s="57" t="n">
         <v>20</v>
       </c>
-      <c r="E9" s="57" t="s">
+      <c r="E9" s="58" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="54"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="55" t="s">
+      <c r="B10" s="55"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="56" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="54"/>
-      <c r="C11" s="55"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="55" t="s">
+      <c r="B11" s="55"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="56" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="54"/>
-      <c r="C12" s="58" t="s">
+      <c r="B12" s="55"/>
+      <c r="C12" s="59" t="s">
         <v>202</v>
       </c>
-      <c r="D12" s="59" t="n">
+      <c r="D12" s="60" t="n">
         <v>20</v>
       </c>
-      <c r="E12" s="60" t="s">
+      <c r="E12" s="61" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="54"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="60" t="s">
+      <c r="B13" s="55"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="61" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="54"/>
-      <c r="C14" s="58"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="58" t="s">
+      <c r="B14" s="55"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="59" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="54"/>
-      <c r="C15" s="61" t="s">
+      <c r="B15" s="55"/>
+      <c r="C15" s="62" t="s">
         <v>206</v>
       </c>
-      <c r="D15" s="56" t="n">
+      <c r="D15" s="57" t="n">
         <v>20</v>
       </c>
-      <c r="E15" s="57" t="s">
+      <c r="E15" s="58" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="54"/>
-      <c r="C16" s="61"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="62" t="s">
+      <c r="B16" s="55"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="63" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="54"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="62" t="s">
+      <c r="B17" s="55"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="63" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="54"/>
-      <c r="C18" s="61"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="62" t="s">
+      <c r="B18" s="55"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="63" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="54"/>
-      <c r="C19" s="63" t="s">
+      <c r="B19" s="55"/>
+      <c r="C19" s="64" t="s">
         <v>211</v>
       </c>
-      <c r="D19" s="59" t="n">
+      <c r="D19" s="60" t="n">
         <v>20</v>
       </c>
-      <c r="E19" s="60" t="s">
+      <c r="E19" s="61" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="54"/>
-      <c r="C20" s="63"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="60" t="s">
+      <c r="B20" s="55"/>
+      <c r="C20" s="64"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="61" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="54"/>
-      <c r="C21" s="63"/>
-      <c r="D21" s="59"/>
-      <c r="E21" s="60"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="60"/>
+      <c r="E21" s="61"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="54"/>
-      <c r="C22" s="64" t="s">
+      <c r="B22" s="55"/>
+      <c r="C22" s="65" t="s">
         <v>214</v>
       </c>
-      <c r="D22" s="56" t="n">
+      <c r="D22" s="57" t="n">
         <v>20</v>
       </c>
-      <c r="E22" s="57" t="s">
+      <c r="E22" s="58" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="54"/>
-      <c r="C23" s="64"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="57" t="s">
+      <c r="B23" s="55"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="58" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="65" t="s">
+      <c r="B25" s="66" t="s">
         <v>217</v>
       </c>
-      <c r="C25" s="66"/>
-      <c r="D25" s="67" t="n">
+      <c r="C25" s="67"/>
+      <c r="D25" s="68" t="n">
         <f aca="false">SUM(D9:D24)</f>
         <v>100</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="53" t="s">
+      <c r="C27" s="54" t="s">
         <v>218</v>
       </c>
-      <c r="D27" s="52" t="s">
+      <c r="D27" s="53" t="s">
         <v>195</v>
       </c>
-      <c r="E27" s="53" t="s">
+      <c r="E27" s="54" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C28" s="64" t="s">
+      <c r="C28" s="65" t="s">
         <v>219</v>
       </c>
-      <c r="D28" s="56" t="n">
+      <c r="D28" s="57" t="n">
         <v>100</v>
       </c>
-      <c r="E28" s="57" t="s">
+      <c r="E28" s="58" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="64"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="62" t="s">
+      <c r="C29" s="65"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="63" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="64"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="62" t="s">
+      <c r="C30" s="65"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="63" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="64"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="62" t="s">
+      <c r="C31" s="65"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="63" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="64"/>
-      <c r="D32" s="56"/>
-      <c r="E32" s="62" t="s">
+      <c r="C32" s="65"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="63" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D33" s="68"/>
+      <c r="D33" s="69"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D34" s="68"/>
+      <c r="D34" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3733,7 +3842,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3743,393 +3852,393 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="70.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="101.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="1.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="70.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="101.85"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="70" t="s">
         <v>225</v>
       </c>
-      <c r="F2" s="70" t="s">
+      <c r="F2" s="71" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F3" s="70" t="s">
+      <c r="F3" s="71" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="53" t="s">
+    <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="54" t="s">
         <v>194</v>
       </c>
-      <c r="C4" s="52" t="s">
+      <c r="C4" s="53" t="s">
         <v>195</v>
       </c>
-      <c r="D4" s="71" t="s">
+      <c r="D4" s="72" t="s">
         <v>228</v>
       </c>
-      <c r="E4" s="53" t="s">
+      <c r="E4" s="54" t="s">
         <v>229</v>
       </c>
-      <c r="F4" s="53" t="s">
+      <c r="F4" s="54" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="73" t="s">
         <v>198</v>
       </c>
-      <c r="C5" s="56" t="n">
+      <c r="C5" s="57" t="n">
         <v>20</v>
       </c>
-      <c r="D5" s="56" t="n">
+      <c r="D5" s="57" t="n">
         <v>7</v>
       </c>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="58" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="72"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="55" t="s">
+      <c r="B6" s="73"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="56" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="72"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="55" t="s">
+      <c r="B7" s="73"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="56" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="73" t="s">
+      <c r="B8" s="74" t="s">
         <v>202</v>
       </c>
-      <c r="C8" s="59" t="n">
+      <c r="C8" s="60" t="n">
         <v>20</v>
       </c>
-      <c r="D8" s="59" t="n">
+      <c r="D8" s="60" t="n">
         <v>7</v>
       </c>
-      <c r="E8" s="60" t="s">
+      <c r="E8" s="61" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="73"/>
-      <c r="C9" s="59"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="60" t="s">
+      <c r="B9" s="74"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="61" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="73"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="58" t="s">
+      <c r="B10" s="74"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="59" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="75" t="s">
         <v>206</v>
       </c>
-      <c r="C11" s="56" t="n">
+      <c r="C11" s="57" t="n">
         <v>20</v>
       </c>
-      <c r="D11" s="75" t="n">
+      <c r="D11" s="76" t="n">
         <v>7</v>
       </c>
-      <c r="E11" s="57" t="s">
+      <c r="E11" s="58" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="74"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="75"/>
-      <c r="E12" s="62" t="s">
+      <c r="B12" s="75"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="63" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="74"/>
-      <c r="C13" s="56"/>
-      <c r="D13" s="75"/>
-      <c r="E13" s="62" t="s">
+      <c r="B13" s="75"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="76"/>
+      <c r="E13" s="63" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="74"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="75"/>
-      <c r="E14" s="62" t="s">
+      <c r="B14" s="75"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="63" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="76" t="s">
+      <c r="B15" s="77" t="s">
         <v>231</v>
       </c>
-      <c r="C15" s="59" t="n">
+      <c r="C15" s="60" t="n">
         <v>20</v>
       </c>
-      <c r="D15" s="77" t="n">
+      <c r="D15" s="78" t="n">
         <v>7</v>
       </c>
-      <c r="E15" s="60" t="s">
+      <c r="E15" s="61" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="76"/>
-      <c r="C16" s="59"/>
-      <c r="D16" s="77"/>
-      <c r="E16" s="60" t="s">
+      <c r="B16" s="77"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="61" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="78" t="s">
+      <c r="B17" s="79" t="s">
         <v>232</v>
       </c>
-      <c r="C17" s="56" t="n">
+      <c r="C17" s="57" t="n">
         <v>20</v>
       </c>
-      <c r="D17" s="79" t="n">
+      <c r="D17" s="80" t="n">
         <v>7</v>
       </c>
-      <c r="E17" s="57" t="s">
+      <c r="E17" s="58" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="78"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="79"/>
-      <c r="E18" s="57" t="s">
+      <c r="B18" s="79"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="80"/>
+      <c r="E18" s="58" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="80" t="s">
+      <c r="B19" s="81" t="s">
         <v>235</v>
       </c>
-      <c r="C19" s="80"/>
-      <c r="D19" s="80"/>
-      <c r="E19" s="80"/>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="81" t="n">
+      <c r="C19" s="81"/>
+      <c r="D19" s="81"/>
+      <c r="E19" s="81"/>
+    </row>
+    <row r="20" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="82" t="n">
         <f aca="false">SUM(C5:C18)</f>
         <v>100</v>
       </c>
-      <c r="D20" s="82" t="n">
+      <c r="D20" s="83" t="n">
         <f aca="false">(D5*C5+D8*C8+D11*C11+D15*C15+D17*C17)/C20</f>
         <v>7</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="69" t="s">
+      <c r="B22" s="70" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="53" t="s">
+      <c r="B24" s="54" t="s">
         <v>237</v>
       </c>
-      <c r="C24" s="52" t="s">
+      <c r="C24" s="53" t="s">
         <v>238</v>
       </c>
-      <c r="D24" s="83" t="s">
+      <c r="D24" s="84" t="s">
         <v>239</v>
       </c>
-      <c r="E24" s="53" t="s">
+      <c r="E24" s="54" t="s">
         <v>240</v>
       </c>
-      <c r="F24" s="53" t="s">
+      <c r="F24" s="54" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C25" s="0" t="n">
+      <c r="C25" s="1" t="n">
         <v>123456</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="D25" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="E25" s="84" t="n">
+      <c r="E25" s="85" t="n">
         <f aca="false">$D$20*D25/$D$34</f>
         <v>7</v>
       </c>
-      <c r="F25" s="0" t="s">
+      <c r="F25" s="1" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C26" s="0" t="n">
+      <c r="C26" s="1" t="n">
         <v>123456</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D26" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="E26" s="84" t="n">
+      <c r="E26" s="85" t="n">
         <f aca="false">$D$20*D26/$D$34</f>
         <v>7</v>
       </c>
-      <c r="F26" s="0" t="s">
+      <c r="F26" s="1" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C27" s="0" t="n">
+      <c r="C27" s="1" t="n">
         <v>123456</v>
       </c>
-      <c r="D27" s="0" t="n">
+      <c r="D27" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="E27" s="84" t="n">
+      <c r="E27" s="85" t="n">
         <f aca="false">$D$20*D27/$D$34</f>
         <v>7</v>
       </c>
-      <c r="F27" s="0" t="s">
+      <c r="F27" s="1" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C28" s="0" t="n">
+      <c r="C28" s="1" t="n">
         <v>123456</v>
       </c>
-      <c r="D28" s="0" t="n">
+      <c r="D28" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="E28" s="84" t="n">
+      <c r="E28" s="85" t="n">
         <f aca="false">$D$20*D28/$D$34</f>
         <v>7</v>
       </c>
-      <c r="F28" s="0" t="s">
+      <c r="F28" s="1" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C29" s="0" t="n">
+      <c r="C29" s="1" t="n">
         <v>123456</v>
       </c>
-      <c r="D29" s="0" t="n">
+      <c r="D29" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="E29" s="84" t="n">
+      <c r="E29" s="85" t="n">
         <f aca="false">$D$20*D29/$D$34</f>
         <v>7</v>
       </c>
-      <c r="F29" s="0" t="s">
+      <c r="F29" s="1" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C30" s="0" t="n">
+      <c r="C30" s="1" t="n">
         <v>123456</v>
       </c>
-      <c r="D30" s="0" t="n">
+      <c r="D30" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="E30" s="84" t="n">
+      <c r="E30" s="85" t="n">
         <f aca="false">$D$20*D30/$D$34</f>
         <v>7</v>
       </c>
-      <c r="F30" s="0" t="s">
+      <c r="F30" s="1" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C31" s="0" t="n">
+      <c r="C31" s="1" t="n">
         <v>123456</v>
       </c>
-      <c r="D31" s="0" t="n">
+      <c r="D31" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="E31" s="84" t="n">
+      <c r="E31" s="85" t="n">
         <f aca="false">$D$20*D31/$D$34</f>
         <v>7</v>
       </c>
-      <c r="F31" s="0" t="s">
+      <c r="F31" s="1" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C32" s="0" t="n">
+      <c r="C32" s="1" t="n">
         <v>123456</v>
       </c>
-      <c r="D32" s="0" t="n">
+      <c r="D32" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="E32" s="84" t="n">
+      <c r="E32" s="85" t="n">
         <f aca="false">$D$20*D32/$D$34</f>
         <v>7</v>
       </c>
-      <c r="F32" s="0" t="s">
+      <c r="F32" s="1" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="85" t="s">
+      <c r="C34" s="86" t="s">
         <v>244</v>
       </c>
-      <c r="D34" s="0" t="n">
+      <c r="D34" s="1" t="n">
         <f aca="false">AVERAGE(D25:D32)</f>
         <v>7</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="1" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="1" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="1" t="s">
         <v>247</v>
       </c>
     </row>
@@ -4163,620 +4272,620 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="B2:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E42" activeCellId="0" sqref="E42"/>
+      <selection pane="topLeft" activeCell="E53" activeCellId="0" sqref="E53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="70.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="101.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="1.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="70.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="101.85"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="70" t="s">
         <v>248</v>
       </c>
-      <c r="F2" s="70" t="s">
+      <c r="F2" s="71" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F3" s="70" t="s">
+      <c r="F3" s="71" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="53" t="s">
+    <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="54" t="s">
         <v>194</v>
       </c>
-      <c r="C4" s="52" t="s">
+      <c r="C4" s="53" t="s">
         <v>195</v>
       </c>
-      <c r="D4" s="71" t="s">
+      <c r="D4" s="72" t="s">
         <v>249</v>
       </c>
-      <c r="E4" s="53" t="s">
+      <c r="E4" s="54" t="s">
         <v>229</v>
       </c>
-      <c r="F4" s="53" t="s">
+      <c r="F4" s="54" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="73" t="s">
         <v>198</v>
       </c>
-      <c r="C5" s="56" t="n">
+      <c r="C5" s="57" t="n">
         <v>20</v>
       </c>
-      <c r="D5" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="57" t="s">
+      <c r="D5" s="80" t="n">
+        <v>9</v>
+      </c>
+      <c r="E5" s="58" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="72"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="55" t="s">
+      <c r="B6" s="73"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="56" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="72"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="55" t="s">
+      <c r="B7" s="73"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="80"/>
+      <c r="E7" s="56" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="73" t="s">
+      <c r="B8" s="74" t="s">
         <v>202</v>
       </c>
-      <c r="C8" s="59" t="n">
+      <c r="C8" s="60" t="n">
         <v>20</v>
       </c>
-      <c r="D8" s="77" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="60" t="s">
+      <c r="D8" s="78" t="n">
+        <v>9</v>
+      </c>
+      <c r="E8" s="61" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="73"/>
-      <c r="C9" s="59"/>
-      <c r="D9" s="77"/>
-      <c r="E9" s="60" t="s">
+      <c r="B9" s="74"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="61" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="73"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="77"/>
-      <c r="E10" s="58" t="s">
+      <c r="B10" s="74"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="59" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="75" t="s">
         <v>206</v>
       </c>
-      <c r="C11" s="56" t="n">
+      <c r="C11" s="57" t="n">
         <v>20</v>
       </c>
-      <c r="D11" s="86" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" s="57" t="s">
+      <c r="D11" s="87" t="n">
+        <v>9</v>
+      </c>
+      <c r="E11" s="58" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="74"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="62" t="s">
+      <c r="B12" s="75"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="87"/>
+      <c r="E12" s="63" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="74"/>
-      <c r="C13" s="56"/>
-      <c r="D13" s="86"/>
-      <c r="E13" s="62" t="s">
+      <c r="B13" s="75"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="87"/>
+      <c r="E13" s="63" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="74"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="86"/>
-      <c r="E14" s="62" t="s">
+      <c r="B14" s="75"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="87"/>
+      <c r="E14" s="63" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="76" t="s">
+      <c r="B15" s="77" t="s">
         <v>231</v>
       </c>
-      <c r="C15" s="59" t="n">
+      <c r="C15" s="60" t="n">
         <v>20</v>
       </c>
-      <c r="D15" s="77" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" s="60" t="s">
+      <c r="D15" s="78" t="n">
+        <v>10</v>
+      </c>
+      <c r="E15" s="61" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="76"/>
-      <c r="C16" s="59"/>
-      <c r="D16" s="77"/>
-      <c r="E16" s="60" t="s">
+      <c r="B16" s="77"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="61" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="78" t="s">
+      <c r="B17" s="79" t="s">
         <v>232</v>
       </c>
-      <c r="C17" s="56" t="n">
+      <c r="C17" s="57" t="n">
         <v>20</v>
       </c>
-      <c r="D17" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="E17" s="57" t="s">
+      <c r="D17" s="80" t="n">
+        <v>9</v>
+      </c>
+      <c r="E17" s="58" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="78"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="79"/>
-      <c r="E18" s="57" t="s">
+    <row r="18" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="79"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="80"/>
+      <c r="E18" s="58" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="80" t="s">
+      <c r="B19" s="81" t="s">
         <v>251</v>
       </c>
-      <c r="C19" s="80"/>
-      <c r="D19" s="80"/>
-      <c r="E19" s="80"/>
-    </row>
-    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="81" t="n">
+      <c r="C19" s="81"/>
+      <c r="D19" s="81"/>
+      <c r="E19" s="81"/>
+    </row>
+    <row r="20" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="82" t="n">
         <f aca="false">SUM(C5:C18)</f>
         <v>100</v>
       </c>
-      <c r="D20" s="82" t="n">
+      <c r="D20" s="83" t="n">
         <f aca="false">(D5*C5+D8*C8+D11*C11+D15*C15+D17*C17)/C20</f>
-        <v>0</v>
+        <v>9.2</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="70" t="s">
+      <c r="B22" s="71" t="s">
         <v>252</v>
       </c>
-      <c r="F22" s="87" t="s">
+      <c r="F22" s="88" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="70" t="s">
+      <c r="B23" s="71" t="s">
         <v>254</v>
       </c>
-      <c r="F23" s="88"/>
+      <c r="F23" s="89"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F24" s="88"/>
+      <c r="F24" s="89"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C25" s="89" t="s">
+      <c r="C25" s="90" t="s">
         <v>255</v>
       </c>
-      <c r="D25" s="89"/>
-      <c r="F25" s="88"/>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="90" t="s">
+      <c r="D25" s="90"/>
+      <c r="F25" s="89"/>
+    </row>
+    <row r="26" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="91" t="s">
         <v>256</v>
       </c>
-      <c r="C26" s="89" t="s">
+      <c r="C26" s="90" t="s">
         <v>257</v>
       </c>
-      <c r="D26" s="89" t="s">
+      <c r="D26" s="90" t="s">
         <v>258</v>
       </c>
-      <c r="E26" s="91" t="s">
+      <c r="E26" s="92" t="s">
         <v>259</v>
       </c>
-      <c r="F26" s="88"/>
+      <c r="F26" s="89"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0" t="n">
+      <c r="B27" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E27" s="0" t="s">
+      <c r="E27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F27" s="88"/>
+      <c r="F27" s="89"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="n">
+      <c r="B28" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E28" s="0" t="s">
+      <c r="E28" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F28" s="88"/>
+      <c r="F28" s="89"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="n">
+      <c r="B29" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E29" s="0" t="s">
+      <c r="E29" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="88"/>
+      <c r="F29" s="89"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0" t="n">
+      <c r="B30" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C30" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E30" s="0" t="s">
+      <c r="E30" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F30" s="88"/>
+      <c r="F30" s="89"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0" t="n">
+      <c r="B31" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E31" s="0" t="s">
+      <c r="E31" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F31" s="88"/>
+      <c r="F31" s="89"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="n">
+      <c r="B32" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E32" s="0" t="s">
+      <c r="E32" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F32" s="88"/>
+      <c r="F32" s="89"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0" t="n">
+      <c r="B33" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="C33" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E33" s="0" t="s">
+      <c r="E33" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="F33" s="88"/>
+      <c r="F33" s="89"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0" t="n">
+      <c r="B34" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="C34" s="0" t="s">
+      <c r="C34" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E34" s="0" t="s">
+      <c r="E34" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F34" s="88"/>
+      <c r="F34" s="89"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0" t="n">
+      <c r="B35" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="C35" s="0" t="s">
+      <c r="C35" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E35" s="0" t="s">
+      <c r="E35" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F35" s="88"/>
+      <c r="F35" s="89"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="0" t="n">
+      <c r="B36" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="C36" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E36" s="0" t="s">
+      <c r="E36" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F36" s="88"/>
+      <c r="F36" s="89"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="0" t="n">
+      <c r="B37" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="C37" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E37" s="0" t="s">
+      <c r="E37" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F37" s="88"/>
+      <c r="F37" s="89"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="0" t="n">
+      <c r="B38" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="C38" s="0" t="s">
+      <c r="C38" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E38" s="0" t="s">
+      <c r="E38" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F38" s="88"/>
+      <c r="F38" s="89"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="0" t="n">
+      <c r="B39" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="C39" s="0" t="s">
+      <c r="C39" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E39" s="0" t="s">
+      <c r="E39" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F39" s="88"/>
+      <c r="F39" s="89"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="0" t="n">
+      <c r="B40" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="C40" s="0" t="s">
+      <c r="C40" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E40" s="0" t="s">
+      <c r="E40" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F40" s="88"/>
+      <c r="F40" s="89"/>
     </row>
     <row r="41" customFormat="false" ht="5.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B41" s="92"/>
-      <c r="C41" s="92"/>
-      <c r="D41" s="92"/>
-      <c r="E41" s="92"/>
-      <c r="F41" s="88"/>
+      <c r="B41" s="93"/>
+      <c r="C41" s="93"/>
+      <c r="D41" s="93"/>
+      <c r="E41" s="93"/>
+      <c r="F41" s="89"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="0" t="n">
+      <c r="B42" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="C42" s="0" t="s">
+      <c r="C42" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E42" s="0" t="s">
+      <c r="E42" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="F42" s="88"/>
+      <c r="F42" s="89"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="0" t="n">
+      <c r="B43" s="1" t="n">
         <v>102</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="C43" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="E43" s="0" t="s">
+      <c r="E43" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="F43" s="88"/>
+      <c r="F43" s="89"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="0" t="n">
+      <c r="B44" s="1" t="n">
         <v>103</v>
       </c>
-      <c r="C44" s="0" t="s">
+      <c r="C44" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="E44" s="0" t="s">
+      <c r="E44" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="F44" s="88"/>
+      <c r="F44" s="89"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="0" t="n">
+      <c r="B45" s="1" t="n">
         <v>104</v>
       </c>
-      <c r="C45" s="0" t="s">
+      <c r="C45" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="E45" s="0" t="s">
+      <c r="E45" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="F45" s="88"/>
+      <c r="F45" s="89"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="0" t="n">
+      <c r="B46" s="1" t="n">
         <v>105</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="C46" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="E46" s="0" t="s">
+      <c r="E46" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="F46" s="88"/>
+      <c r="F46" s="89"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0" t="n">
+      <c r="B47" s="1" t="n">
         <v>106</v>
       </c>
-      <c r="C47" s="0" t="s">
+      <c r="C47" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E47" s="0" t="s">
+      <c r="E47" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="F47" s="88"/>
+      <c r="F47" s="89"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="69" t="s">
+      <c r="B49" s="70" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="53" t="s">
+      <c r="B51" s="54" t="s">
         <v>237</v>
       </c>
-      <c r="C51" s="52" t="s">
+      <c r="C51" s="53" t="s">
         <v>238</v>
       </c>
-      <c r="D51" s="83" t="s">
+      <c r="D51" s="84" t="s">
         <v>239</v>
       </c>
-      <c r="E51" s="53" t="s">
+      <c r="E51" s="54" t="s">
         <v>270</v>
       </c>
-      <c r="F51" s="53" t="s">
+      <c r="F51" s="54" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="0" t="s">
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="C52" s="0" t="n">
+      <c r="C52" s="1" t="n">
         <v>2183499</v>
       </c>
-      <c r="D52" s="0" t="n">
+      <c r="D52" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="E52" s="84" t="n">
+      <c r="E52" s="85" t="n">
         <f aca="false">$D$20*D52/$D$58</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="0" t="s">
+        <v>10.0821917808219</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="C53" s="0" t="n">
+      <c r="C53" s="1" t="n">
         <v>2184122</v>
       </c>
-      <c r="D53" s="0" t="n">
+      <c r="D53" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="E53" s="84" t="n">
+      <c r="E53" s="85" t="n">
         <f aca="false">$D$20*D53/$D$58</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="0" t="s">
+        <v>10.0821917808219</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="C54" s="0" t="n">
+      <c r="C54" s="1" t="n">
         <v>2184441</v>
       </c>
-      <c r="D54" s="0" t="n">
+      <c r="D54" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="E54" s="84" t="n">
+      <c r="E54" s="85" t="n">
         <f aca="false">$D$20*D54/$D$58</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="0" t="s">
+        <v>10.0821917808219</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="C55" s="0" t="n">
+      <c r="C55" s="1" t="n">
         <v>2177643</v>
       </c>
-      <c r="D55" s="0" t="n">
+      <c r="D55" s="1" t="n">
         <v>6.5</v>
       </c>
-      <c r="E55" s="84" t="n">
+      <c r="E55" s="85" t="n">
         <f aca="false">$D$20*D55/$D$58</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="0" t="s">
+        <v>8.19178082191781</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="C56" s="0" t="n">
+      <c r="C56" s="1" t="n">
         <v>2154689</v>
       </c>
-      <c r="D56" s="0" t="n">
+      <c r="D56" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="E56" s="84" t="n">
+      <c r="E56" s="85" t="n">
         <f aca="false">$D$20*D56/$D$58</f>
-        <v>0</v>
+        <v>7.56164383561644</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C58" s="85" t="s">
+      <c r="C58" s="86" t="s">
         <v>244</v>
       </c>
-      <c r="D58" s="0" t="n">
+      <c r="D58" s="1" t="n">
         <f aca="false">AVERAGE(D52:D56)</f>
         <v>7.3</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="0" t="s">
+      <c r="B60" s="1" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="0" t="s">
+      <c r="B61" s="1" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="0" t="s">
+      <c r="B62" s="1" t="s">
         <v>247</v>
       </c>
     </row>
@@ -4815,7 +4924,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -4825,54 +4934,54 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="122.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="122.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="93" t="s">
+      <c r="B2" s="94" t="s">
         <v>277</v>
       </c>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
     </row>
     <row r="3" customFormat="false" ht="5.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="70" t="s">
         <v>278</v>
       </c>
-      <c r="C4" s="69" t="s">
+      <c r="C4" s="70" t="s">
         <v>279</v>
       </c>
-      <c r="D4" s="69" t="s">
+      <c r="D4" s="70" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="94" t="n">
+      <c r="B5" s="95" t="n">
         <v>45527</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="95" t="s">
+      <c r="D5" s="96" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="96"/>
-      <c r="C7" s="85"/>
+      <c r="B7" s="97"/>
+      <c r="C7" s="86"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="94"/>
+      <c r="B8" s="95"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>